<commit_message>
Se realizarón los cambios propuestos al archivo index.html (texto).
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506FDDD9-69FC-4FD6-9152-06F15F0F007F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA20673-9D77-406E-8080-313185E25908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="146">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -452,6 +452,18 @@
   </si>
   <si>
     <t xml:space="preserve">18:30 - 19:30 </t>
+  </si>
+  <si>
+    <t>SEMANA 23</t>
+  </si>
+  <si>
+    <t>Se realizarón los cambio solicitados en index.html</t>
+  </si>
+  <si>
+    <t>Correcciónes de texto y ocultación de elementos</t>
+  </si>
+  <si>
+    <t>19:00-18:30</t>
   </si>
 </sst>
 </file>
@@ -608,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -659,6 +671,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -943,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="F211" sqref="F211"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="F221" sqref="F221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,7 +983,7 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45782</v>
+        <v>45798</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
@@ -1007,7 +1028,7 @@
       </c>
       <c r="J6" s="17">
         <f>SUM(G12:G1202)</f>
-        <v>292.7</v>
+        <v>294.2</v>
       </c>
       <c r="K6" s="17"/>
     </row>
@@ -1064,7 +1085,7 @@
       </c>
       <c r="J9" s="11">
         <f>460-J6</f>
-        <v>167.3</v>
+        <v>165.8</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1085,7 +1106,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>41.825000000000003</v>
+        <v>41.45</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1106,7 +1127,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>1.045625</v>
+        <v>1.0362500000000001</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -3541,120 +3562,150 @@
       </c>
     </row>
     <row r="211" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B211" s="7"/>
-      <c r="C211" s="3"/>
-      <c r="D211" s="3"/>
-      <c r="E211" s="3"/>
-      <c r="F211" s="3"/>
-    </row>
-    <row r="212" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B212" s="7"/>
-      <c r="C212" s="3"/>
-      <c r="D212" s="3"/>
-      <c r="E212" s="3"/>
-      <c r="F212" s="3"/>
-      <c r="G212" s="9" t="s">
+      <c r="B211"/>
+      <c r="C211"/>
+      <c r="D211"/>
+      <c r="E211"/>
+      <c r="F211"/>
+      <c r="G211" s="4">
+        <f>SUM(F210)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B213" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C213" s="19"/>
+      <c r="D213" s="19"/>
+      <c r="E213" s="19"/>
+      <c r="F213" s="20"/>
+    </row>
+    <row r="214" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B214" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D214" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F214" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B215" s="7">
+        <v>45782</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F215" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="216" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B216"/>
+      <c r="C216"/>
+      <c r="D216"/>
+      <c r="E216"/>
+      <c r="F216"/>
+      <c r="G216" s="4">
+        <f>SUM(F215)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="217" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B217"/>
+      <c r="C217"/>
+      <c r="D217"/>
+      <c r="E217"/>
+      <c r="F217"/>
+      <c r="G217" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="213" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B213" s="7"/>
-      <c r="C213" s="3"/>
-      <c r="D213" s="3"/>
-      <c r="E213" s="3"/>
-      <c r="F213" s="3"/>
-    </row>
-    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B214" s="7"/>
-      <c r="C214" s="3"/>
-      <c r="D214" s="3"/>
-      <c r="E214" s="3"/>
-      <c r="F214" s="3"/>
-    </row>
-    <row r="215" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B215"/>
-      <c r="C215"/>
-      <c r="D215"/>
-      <c r="E215"/>
-      <c r="F215"/>
-      <c r="G215" s="4">
-        <f>SUM(F210:F215)</f>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B218" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C218" s="19"/>
+      <c r="D218" s="19"/>
+      <c r="E218" s="19"/>
+      <c r="F218" s="20"/>
+    </row>
+    <row r="219" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B219" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E219" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F219" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B217" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C217" s="12"/>
-      <c r="D217" s="12"/>
-      <c r="E217" s="12"/>
-      <c r="F217" s="12"/>
-    </row>
-    <row r="218" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B218" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D218" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E218" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F218" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B219" s="7">
-        <v>45782</v>
-      </c>
-      <c r="C219" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D219" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="E219" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F219" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B220" s="7"/>
-      <c r="C220" s="3"/>
-      <c r="D220" s="3"/>
-      <c r="E220" s="3"/>
-      <c r="F220" s="3"/>
+    <row r="220" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B220" s="7">
+        <v>45797</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F220" s="3">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="221" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B221" s="7"/>
-      <c r="C221" s="3"/>
-      <c r="D221" s="3"/>
-      <c r="E221" s="3"/>
-      <c r="F221" s="3"/>
-      <c r="G221" s="9" t="s">
+      <c r="B221"/>
+      <c r="C221"/>
+      <c r="D221"/>
+      <c r="E221"/>
+      <c r="F221"/>
+      <c r="G221" s="4">
+        <f>SUM(F220)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="222" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B222"/>
+      <c r="C222"/>
+      <c r="D222"/>
+      <c r="E222"/>
+      <c r="F222"/>
+      <c r="G222" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="222" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B222" s="7"/>
-      <c r="C222" s="3"/>
-      <c r="D222" s="3"/>
-      <c r="E222" s="3"/>
-      <c r="F222" s="3"/>
-    </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B223" s="7"/>
-      <c r="C223" s="3"/>
-      <c r="D223" s="3"/>
-      <c r="E223" s="3"/>
-      <c r="F223" s="3"/>
+      <c r="B223"/>
+      <c r="C223"/>
+      <c r="D223"/>
+      <c r="E223"/>
+      <c r="F223"/>
     </row>
     <row r="224" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B224"/>
@@ -3662,29 +3713,26 @@
       <c r="D224"/>
       <c r="E224"/>
       <c r="F224"/>
-      <c r="G224" s="4">
-        <f>SUM(F219:F224)</f>
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B217:F217"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B89:F89"/>
+  <mergeCells count="28">
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B44:F44"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B71:F71"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B89:F89"/>
     <mergeCell ref="B189:F189"/>
     <mergeCell ref="B98:F98"/>
     <mergeCell ref="B107:F107"/>

</xml_diff>

<commit_message>
Se agregarón los cambios en el menú, solucionando los bugs; También se agregarón los JS's para el Calendario Ambiental
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA20673-9D77-406E-8080-313185E25908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF7B908-FD31-49F6-A2D9-738CE3978BCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="150">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -464,6 +464,18 @@
   </si>
   <si>
     <t>19:00-18:30</t>
+  </si>
+  <si>
+    <t>SEMANA 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se realizarón los cambios en el navbar </t>
+  </si>
+  <si>
+    <t>Corrección en bug de barra y letras en negritas</t>
+  </si>
+  <si>
+    <t>15:00 - 20:30</t>
   </si>
 </sst>
 </file>
@@ -655,7 +667,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -673,13 +691,7 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -962,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N224"/>
+  <dimension ref="B1:N226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="F221" sqref="F221"/>
+    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="E228" sqref="E228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,32 +995,32 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45798</v>
+        <v>45811</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="J5" s="16" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="J5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="16"/>
+      <c r="K5" s="18"/>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1026,11 +1038,11 @@
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="19">
         <f>SUM(G12:G1202)</f>
-        <v>294.2</v>
-      </c>
-      <c r="K6" s="17"/>
+        <v>299.7</v>
+      </c>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
@@ -1085,7 +1097,7 @@
       </c>
       <c r="J9" s="11">
         <f>460-J6</f>
-        <v>165.8</v>
+        <v>160.30000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1106,7 +1118,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>41.45</v>
+        <v>40.075000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1127,7 +1139,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>1.0362500000000001</v>
+        <v>1.0018750000000001</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -1138,13 +1150,13 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1256,13 +1268,13 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1391,13 +1403,13 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
     </row>
     <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -1509,13 +1521,13 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
     </row>
     <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -1627,13 +1639,13 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
     </row>
     <row r="54" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -1745,13 +1757,13 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
     </row>
     <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -1863,13 +1875,13 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
     </row>
     <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -1981,13 +1993,13 @@
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
     </row>
     <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
@@ -2083,13 +2095,13 @@
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="20"/>
     </row>
     <row r="90" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -2161,13 +2173,13 @@
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="12" t="s">
+      <c r="B98" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="20"/>
     </row>
     <row r="99" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -2247,13 +2259,13 @@
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="12" t="s">
+      <c r="B107" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="20"/>
+      <c r="E107" s="20"/>
+      <c r="F107" s="20"/>
     </row>
     <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -2349,13 +2361,13 @@
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="12" t="s">
+      <c r="B116" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
+      <c r="C116" s="20"/>
+      <c r="D116" s="20"/>
+      <c r="E116" s="20"/>
+      <c r="F116" s="20"/>
     </row>
     <row r="117" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
@@ -2451,13 +2463,13 @@
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="12" t="s">
+      <c r="B125" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C125" s="12"/>
-      <c r="D125" s="12"/>
-      <c r="E125" s="12"/>
-      <c r="F125" s="12"/>
+      <c r="C125" s="20"/>
+      <c r="D125" s="20"/>
+      <c r="E125" s="20"/>
+      <c r="F125" s="20"/>
     </row>
     <row r="126" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
@@ -2555,13 +2567,13 @@
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="12" t="s">
+      <c r="B134" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C134" s="12"/>
-      <c r="D134" s="12"/>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12"/>
+      <c r="C134" s="20"/>
+      <c r="D134" s="20"/>
+      <c r="E134" s="20"/>
+      <c r="F134" s="20"/>
     </row>
     <row r="135" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
@@ -2657,13 +2669,13 @@
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="12" t="s">
+      <c r="B143" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C143" s="12"/>
-      <c r="D143" s="12"/>
-      <c r="E143" s="12"/>
-      <c r="F143" s="12"/>
+      <c r="C143" s="20"/>
+      <c r="D143" s="20"/>
+      <c r="E143" s="20"/>
+      <c r="F143" s="20"/>
     </row>
     <row r="144" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
@@ -2784,13 +2796,13 @@
       <c r="N152"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B153" s="12" t="s">
+      <c r="B153" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C153" s="12"/>
-      <c r="D153" s="12"/>
-      <c r="E153" s="12"/>
-      <c r="F153" s="12"/>
+      <c r="C153" s="20"/>
+      <c r="D153" s="20"/>
+      <c r="E153" s="20"/>
+      <c r="F153" s="20"/>
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153"/>
@@ -2904,13 +2916,13 @@
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B162" s="12" t="s">
+      <c r="B162" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C162" s="12"/>
-      <c r="D162" s="12"/>
-      <c r="E162" s="12"/>
-      <c r="F162" s="12"/>
+      <c r="C162" s="20"/>
+      <c r="D162" s="20"/>
+      <c r="E162" s="20"/>
+      <c r="F162" s="20"/>
     </row>
     <row r="163" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
@@ -3039,13 +3051,13 @@
       </c>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B172" s="12" t="s">
+      <c r="B172" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C172" s="12"/>
-      <c r="D172" s="12"/>
-      <c r="E172" s="12"/>
-      <c r="F172" s="12"/>
+      <c r="C172" s="20"/>
+      <c r="D172" s="20"/>
+      <c r="E172" s="20"/>
+      <c r="F172" s="20"/>
     </row>
     <row r="173" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
@@ -3151,13 +3163,13 @@
       <c r="F179"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B180" s="12" t="s">
+      <c r="B180" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C180" s="12"/>
-      <c r="D180" s="12"/>
-      <c r="E180" s="12"/>
-      <c r="F180" s="12"/>
+      <c r="C180" s="20"/>
+      <c r="D180" s="20"/>
+      <c r="E180" s="20"/>
+      <c r="F180" s="20"/>
     </row>
     <row r="181" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
@@ -3277,13 +3289,13 @@
       <c r="D188" s="1"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="12" t="s">
+      <c r="B189" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C189" s="12"/>
-      <c r="D189" s="12"/>
-      <c r="E189" s="12"/>
-      <c r="F189" s="12"/>
+      <c r="C189" s="20"/>
+      <c r="D189" s="20"/>
+      <c r="E189" s="20"/>
+      <c r="F189" s="20"/>
     </row>
     <row r="190" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
@@ -3382,13 +3394,13 @@
       </c>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B198" s="12" t="s">
+      <c r="B198" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C198" s="12"/>
-      <c r="D198" s="12"/>
-      <c r="E198" s="12"/>
-      <c r="F198" s="12"/>
+      <c r="C198" s="20"/>
+      <c r="D198" s="20"/>
+      <c r="E198" s="20"/>
+      <c r="F198" s="20"/>
     </row>
     <row r="199" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
@@ -3519,13 +3531,13 @@
       </c>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B208" s="12" t="s">
+      <c r="B208" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="C208" s="12"/>
-      <c r="D208" s="12"/>
-      <c r="E208" s="12"/>
-      <c r="F208" s="12"/>
+      <c r="C208" s="20"/>
+      <c r="D208" s="20"/>
+      <c r="E208" s="20"/>
+      <c r="F208" s="20"/>
     </row>
     <row r="209" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
@@ -3573,13 +3585,13 @@
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B213" s="18" t="s">
+      <c r="B213" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C213" s="19"/>
-      <c r="D213" s="19"/>
-      <c r="E213" s="19"/>
-      <c r="F213" s="20"/>
+      <c r="C213" s="13"/>
+      <c r="D213" s="13"/>
+      <c r="E213" s="13"/>
+      <c r="F213" s="14"/>
     </row>
     <row r="214" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B214" s="2" t="s">
@@ -3637,13 +3649,13 @@
       </c>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B218" s="18" t="s">
+      <c r="B218" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C218" s="19"/>
-      <c r="D218" s="19"/>
-      <c r="E218" s="19"/>
-      <c r="F218" s="20"/>
+      <c r="C218" s="13"/>
+      <c r="D218" s="13"/>
+      <c r="E218" s="13"/>
+      <c r="F218" s="14"/>
     </row>
     <row r="219" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B219" s="2" t="s">
@@ -3701,21 +3713,74 @@
       </c>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B223"/>
-      <c r="C223"/>
-      <c r="D223"/>
-      <c r="E223"/>
-      <c r="F223"/>
-    </row>
-    <row r="224" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B224"/>
-      <c r="C224"/>
-      <c r="D224"/>
-      <c r="E224"/>
-      <c r="F224"/>
+      <c r="B223" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C223" s="13"/>
+      <c r="D223" s="13"/>
+      <c r="E223" s="13"/>
+      <c r="F223" s="14"/>
+    </row>
+    <row r="224" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B224" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D224" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F224" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B225" s="7">
+        <v>45811</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F225" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="226" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B226"/>
+      <c r="C226"/>
+      <c r="D226"/>
+      <c r="E226"/>
+      <c r="F226"/>
+      <c r="G226" s="4">
+        <f>SUM(F225)</f>
+        <v>5.5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B162:F162"/>
     <mergeCell ref="B213:F213"/>
     <mergeCell ref="B218:F218"/>
     <mergeCell ref="D2:J2"/>
@@ -3732,18 +3797,6 @@
     <mergeCell ref="B198:F198"/>
     <mergeCell ref="B208:F208"/>
     <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B162:F162"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se terminó la imagen principal y la mitad de la parte de contacto en escritorio
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF7B908-FD31-49F6-A2D9-738CE3978BCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DF6C8A-7935-45D2-BFA0-330B69C71A88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOVIEMBRE 2024" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="154">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -476,6 +476,18 @@
   </si>
   <si>
     <t>15:00 - 20:30</t>
+  </si>
+  <si>
+    <t>SEMANA 25</t>
+  </si>
+  <si>
+    <t>Se realzó la primera parte de la maquetación de la página de planta de tratamiento de aguas residuales</t>
+  </si>
+  <si>
+    <t>Seterminó la imagen principal y la mitad de la parte de contacto en escritorio</t>
+  </si>
+  <si>
+    <t>14:00 - 18:30</t>
   </si>
 </sst>
 </file>
@@ -676,6 +688,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -689,9 +704,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -974,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N226"/>
+  <dimension ref="B1:N232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="E228" sqref="E228"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,32 +1007,32 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45811</v>
+        <v>45825</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="J5" s="18" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="J5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="18"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1038,11 +1050,11 @@
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="20">
         <f>SUM(G12:G1202)</f>
-        <v>299.7</v>
-      </c>
-      <c r="K6" s="19"/>
+        <v>304.2</v>
+      </c>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
@@ -1096,8 +1108,8 @@
         <v>1</v>
       </c>
       <c r="J9" s="11">
-        <f>460-J6</f>
-        <v>160.30000000000001</v>
+        <f>480-J6</f>
+        <v>175.8</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1118,7 +1130,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>40.075000000000003</v>
+        <v>43.95</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1139,7 +1151,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>1.0018750000000001</v>
+        <v>1.0987500000000001</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -1150,13 +1162,13 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1268,13 +1280,13 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1403,13 +1415,13 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
     </row>
     <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -1521,13 +1533,13 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
     </row>
     <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -1639,13 +1651,13 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
     </row>
     <row r="54" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -1757,13 +1769,13 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
     </row>
     <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -1875,13 +1887,13 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
     </row>
     <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -1993,13 +2005,13 @@
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
     </row>
     <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
@@ -2095,13 +2107,13 @@
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="20" t="s">
+      <c r="B89" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
     </row>
     <row r="90" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -2173,13 +2185,13 @@
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="20" t="s">
+      <c r="B98" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="20"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="20"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
     </row>
     <row r="99" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -2259,13 +2271,13 @@
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="20" t="s">
+      <c r="B107" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="20"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
     </row>
     <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -2361,13 +2373,13 @@
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="20" t="s">
+      <c r="B116" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C116" s="20"/>
-      <c r="D116" s="20"/>
-      <c r="E116" s="20"/>
-      <c r="F116" s="20"/>
+      <c r="C116" s="15"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
     </row>
     <row r="117" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
@@ -2463,13 +2475,13 @@
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="20" t="s">
+      <c r="B125" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C125" s="20"/>
-      <c r="D125" s="20"/>
-      <c r="E125" s="20"/>
-      <c r="F125" s="20"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
     </row>
     <row r="126" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
@@ -2567,13 +2579,13 @@
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="20" t="s">
+      <c r="B134" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C134" s="20"/>
-      <c r="D134" s="20"/>
-      <c r="E134" s="20"/>
-      <c r="F134" s="20"/>
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
     </row>
     <row r="135" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
@@ -2669,13 +2681,13 @@
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="20" t="s">
+      <c r="B143" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C143" s="20"/>
-      <c r="D143" s="20"/>
-      <c r="E143" s="20"/>
-      <c r="F143" s="20"/>
+      <c r="C143" s="15"/>
+      <c r="D143" s="15"/>
+      <c r="E143" s="15"/>
+      <c r="F143" s="15"/>
     </row>
     <row r="144" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
@@ -2796,13 +2808,13 @@
       <c r="N152"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B153" s="20" t="s">
+      <c r="B153" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C153" s="20"/>
-      <c r="D153" s="20"/>
-      <c r="E153" s="20"/>
-      <c r="F153" s="20"/>
+      <c r="C153" s="15"/>
+      <c r="D153" s="15"/>
+      <c r="E153" s="15"/>
+      <c r="F153" s="15"/>
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153"/>
@@ -2916,13 +2928,13 @@
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B162" s="20" t="s">
+      <c r="B162" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C162" s="20"/>
-      <c r="D162" s="20"/>
-      <c r="E162" s="20"/>
-      <c r="F162" s="20"/>
+      <c r="C162" s="15"/>
+      <c r="D162" s="15"/>
+      <c r="E162" s="15"/>
+      <c r="F162" s="15"/>
     </row>
     <row r="163" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
@@ -3051,13 +3063,13 @@
       </c>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B172" s="20" t="s">
+      <c r="B172" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C172" s="20"/>
-      <c r="D172" s="20"/>
-      <c r="E172" s="20"/>
-      <c r="F172" s="20"/>
+      <c r="C172" s="15"/>
+      <c r="D172" s="15"/>
+      <c r="E172" s="15"/>
+      <c r="F172" s="15"/>
     </row>
     <row r="173" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
@@ -3163,13 +3175,13 @@
       <c r="F179"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B180" s="20" t="s">
+      <c r="B180" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C180" s="20"/>
-      <c r="D180" s="20"/>
-      <c r="E180" s="20"/>
-      <c r="F180" s="20"/>
+      <c r="C180" s="15"/>
+      <c r="D180" s="15"/>
+      <c r="E180" s="15"/>
+      <c r="F180" s="15"/>
     </row>
     <row r="181" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
@@ -3289,13 +3301,13 @@
       <c r="D188" s="1"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="20" t="s">
+      <c r="B189" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C189" s="20"/>
-      <c r="D189" s="20"/>
-      <c r="E189" s="20"/>
-      <c r="F189" s="20"/>
+      <c r="C189" s="15"/>
+      <c r="D189" s="15"/>
+      <c r="E189" s="15"/>
+      <c r="F189" s="15"/>
     </row>
     <row r="190" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
@@ -3394,13 +3406,13 @@
       </c>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B198" s="20" t="s">
+      <c r="B198" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C198" s="20"/>
-      <c r="D198" s="20"/>
-      <c r="E198" s="20"/>
-      <c r="F198" s="20"/>
+      <c r="C198" s="15"/>
+      <c r="D198" s="15"/>
+      <c r="E198" s="15"/>
+      <c r="F198" s="15"/>
     </row>
     <row r="199" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
@@ -3531,13 +3543,13 @@
       </c>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B208" s="20" t="s">
+      <c r="B208" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C208" s="20"/>
-      <c r="D208" s="20"/>
-      <c r="E208" s="20"/>
-      <c r="F208" s="20"/>
+      <c r="C208" s="15"/>
+      <c r="D208" s="15"/>
+      <c r="E208" s="15"/>
+      <c r="F208" s="15"/>
     </row>
     <row r="209" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
@@ -3766,8 +3778,76 @@
         <v>5.5</v>
       </c>
     </row>
+    <row r="229" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B229" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C229" s="13"/>
+      <c r="D229" s="13"/>
+      <c r="E229" s="13"/>
+      <c r="F229" s="14"/>
+    </row>
+    <row r="230" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B230" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D230" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E230" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F230" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B231" s="7">
+        <v>45825</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F231" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="232" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B232"/>
+      <c r="C232"/>
+      <c r="D232"/>
+      <c r="E232"/>
+      <c r="F232"/>
+      <c r="G232" s="4">
+        <f>SUM(F231)</f>
+        <v>4.5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B223:F223"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B189:F189"/>
@@ -3783,20 +3863,7 @@
     <mergeCell ref="B162:F162"/>
     <mergeCell ref="B213:F213"/>
     <mergeCell ref="B218:F218"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
     <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B80:F80"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se terminó la segunda y tercera parte de la pagina para escritorio, tambien se empezó con la tercera sección de la planta de tratamiento AR
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DF6C8A-7935-45D2-BFA0-330B69C71A88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7379CE-4094-4ADC-A3BD-AC86282276C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOVIEMBRE 2024" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="157">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -484,10 +484,19 @@
     <t>Se realzó la primera parte de la maquetación de la página de planta de tratamiento de aguas residuales</t>
   </si>
   <si>
-    <t>Seterminó la imagen principal y la mitad de la parte de contacto en escritorio</t>
-  </si>
-  <si>
     <t>14:00 - 18:30</t>
+  </si>
+  <si>
+    <t>Se terminó la segunda y la tercera parte de la página, para escritorio y se corrigió un error en el footer</t>
+  </si>
+  <si>
+    <t>Se terminó la segunda y tercera parte de la pagina para escritorio, tambien se empezó con la tercera</t>
+  </si>
+  <si>
+    <t>Se terminó la imagen principal y la mitad de la parte de contacto en escritorio</t>
+  </si>
+  <si>
+    <t>8:00 -12:00, 18:00 -21:00</t>
   </si>
 </sst>
 </file>
@@ -679,6 +688,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -686,9 +698,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -986,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N232"/>
+  <dimension ref="B1:N238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="G239" sqref="G239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1016,7 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45825</v>
+        <v>45826</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
@@ -1022,13 +1031,13 @@
       <c r="J2" s="18"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
       <c r="J5" s="19" t="s">
         <v>7</v>
       </c>
@@ -1052,7 +1061,7 @@
       </c>
       <c r="J6" s="20">
         <f>SUM(G12:G1202)</f>
-        <v>304.2</v>
+        <v>311.2</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1109,7 +1118,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>175.8</v>
+        <v>168.8</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1130,7 +1139,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>43.95</v>
+        <v>42.2</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1151,7 +1160,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>1.0987500000000001</v>
+        <v>1.0550000000000002</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -1162,13 +1171,13 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1280,13 +1289,13 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1415,13 +1424,13 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -1533,13 +1542,13 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
     </row>
     <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -1651,13 +1660,13 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
     </row>
     <row r="54" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -1769,13 +1778,13 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
     </row>
     <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -1887,13 +1896,13 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="15"/>
-      <c r="F71" s="15"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
     </row>
     <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -2005,13 +2014,13 @@
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
     </row>
     <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
@@ -2107,13 +2116,13 @@
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="15"/>
-      <c r="F89" s="15"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
     </row>
     <row r="90" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -2185,13 +2194,13 @@
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="15" t="s">
+      <c r="B98" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="15"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="15"/>
-      <c r="F98" s="15"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
     </row>
     <row r="99" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -2271,13 +2280,13 @@
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="15"/>
-      <c r="F107" s="15"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12"/>
     </row>
     <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -2373,13 +2382,13 @@
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="15" t="s">
+      <c r="B116" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="15"/>
-      <c r="E116" s="15"/>
-      <c r="F116" s="15"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
     </row>
     <row r="117" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
@@ -2475,13 +2484,13 @@
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="15" t="s">
+      <c r="B125" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="15"/>
-      <c r="F125" s="15"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
     </row>
     <row r="126" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
@@ -2579,13 +2588,13 @@
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="15" t="s">
+      <c r="B134" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C134" s="15"/>
-      <c r="D134" s="15"/>
-      <c r="E134" s="15"/>
-      <c r="F134" s="15"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
     </row>
     <row r="135" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
@@ -2681,13 +2690,13 @@
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="15" t="s">
+      <c r="B143" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C143" s="15"/>
-      <c r="D143" s="15"/>
-      <c r="E143" s="15"/>
-      <c r="F143" s="15"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="12"/>
     </row>
     <row r="144" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
@@ -2808,13 +2817,13 @@
       <c r="N152"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B153" s="15" t="s">
+      <c r="B153" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C153" s="15"/>
-      <c r="D153" s="15"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
+      <c r="C153" s="12"/>
+      <c r="D153" s="12"/>
+      <c r="E153" s="12"/>
+      <c r="F153" s="12"/>
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153"/>
@@ -2928,13 +2937,13 @@
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B162" s="15" t="s">
+      <c r="B162" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C162" s="15"/>
-      <c r="D162" s="15"/>
-      <c r="E162" s="15"/>
-      <c r="F162" s="15"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="12"/>
+      <c r="E162" s="12"/>
+      <c r="F162" s="12"/>
     </row>
     <row r="163" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
@@ -3063,13 +3072,13 @@
       </c>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B172" s="15" t="s">
+      <c r="B172" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C172" s="15"/>
-      <c r="D172" s="15"/>
-      <c r="E172" s="15"/>
-      <c r="F172" s="15"/>
+      <c r="C172" s="12"/>
+      <c r="D172" s="12"/>
+      <c r="E172" s="12"/>
+      <c r="F172" s="12"/>
     </row>
     <row r="173" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
@@ -3175,13 +3184,13 @@
       <c r="F179"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B180" s="15" t="s">
+      <c r="B180" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C180" s="15"/>
-      <c r="D180" s="15"/>
-      <c r="E180" s="15"/>
-      <c r="F180" s="15"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="12"/>
+      <c r="F180" s="12"/>
     </row>
     <row r="181" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
@@ -3301,13 +3310,13 @@
       <c r="D188" s="1"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="15" t="s">
+      <c r="B189" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C189" s="15"/>
-      <c r="D189" s="15"/>
-      <c r="E189" s="15"/>
-      <c r="F189" s="15"/>
+      <c r="C189" s="12"/>
+      <c r="D189" s="12"/>
+      <c r="E189" s="12"/>
+      <c r="F189" s="12"/>
     </row>
     <row r="190" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
@@ -3406,13 +3415,13 @@
       </c>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B198" s="15" t="s">
+      <c r="B198" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C198" s="15"/>
-      <c r="D198" s="15"/>
-      <c r="E198" s="15"/>
-      <c r="F198" s="15"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="12"/>
+      <c r="E198" s="12"/>
+      <c r="F198" s="12"/>
     </row>
     <row r="199" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
@@ -3543,13 +3552,13 @@
       </c>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B208" s="15" t="s">
+      <c r="B208" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C208" s="15"/>
-      <c r="D208" s="15"/>
-      <c r="E208" s="15"/>
-      <c r="F208" s="15"/>
+      <c r="C208" s="12"/>
+      <c r="D208" s="12"/>
+      <c r="E208" s="12"/>
+      <c r="F208" s="12"/>
     </row>
     <row r="209" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
@@ -3597,13 +3606,13 @@
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B213" s="12" t="s">
+      <c r="B213" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C213" s="13"/>
-      <c r="D213" s="13"/>
-      <c r="E213" s="13"/>
-      <c r="F213" s="14"/>
+      <c r="C213" s="14"/>
+      <c r="D213" s="14"/>
+      <c r="E213" s="14"/>
+      <c r="F213" s="15"/>
     </row>
     <row r="214" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B214" s="2" t="s">
@@ -3661,13 +3670,13 @@
       </c>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B218" s="12" t="s">
+      <c r="B218" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C218" s="13"/>
-      <c r="D218" s="13"/>
-      <c r="E218" s="13"/>
-      <c r="F218" s="14"/>
+      <c r="C218" s="14"/>
+      <c r="D218" s="14"/>
+      <c r="E218" s="14"/>
+      <c r="F218" s="15"/>
     </row>
     <row r="219" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B219" s="2" t="s">
@@ -3725,13 +3734,13 @@
       </c>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B223" s="12" t="s">
+      <c r="B223" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C223" s="13"/>
-      <c r="D223" s="13"/>
-      <c r="E223" s="13"/>
-      <c r="F223" s="14"/>
+      <c r="C223" s="14"/>
+      <c r="D223" s="14"/>
+      <c r="E223" s="14"/>
+      <c r="F223" s="15"/>
     </row>
     <row r="224" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B224" s="2" t="s">
@@ -3779,13 +3788,13 @@
       </c>
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B229" s="12" t="s">
+      <c r="B229" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C229" s="13"/>
-      <c r="D229" s="13"/>
-      <c r="E229" s="13"/>
-      <c r="F229" s="14"/>
+      <c r="C229" s="14"/>
+      <c r="D229" s="14"/>
+      <c r="E229" s="14"/>
+      <c r="F229" s="15"/>
     </row>
     <row r="230" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B230" s="2" t="s">
@@ -3812,28 +3821,99 @@
         <v>151</v>
       </c>
       <c r="D231" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E231" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="E231" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="F231" s="3">
         <v>4.5</v>
       </c>
     </row>
-    <row r="232" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B232"/>
-      <c r="C232"/>
-      <c r="D232"/>
-      <c r="E232"/>
-      <c r="F232"/>
-      <c r="G232" s="4">
-        <f>SUM(F231)</f>
-        <v>4.5</v>
+    <row r="232" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B232" s="7">
+        <v>45826</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F232" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="233" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B233" s="7">
+        <v>45827</v>
+      </c>
+      <c r="C233" s="3"/>
+      <c r="D233" s="3"/>
+      <c r="E233" s="3"/>
+      <c r="F233" s="3"/>
+    </row>
+    <row r="234" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B234" s="7">
+        <v>45828</v>
+      </c>
+      <c r="C234" s="3"/>
+      <c r="D234" s="3"/>
+      <c r="E234" s="3"/>
+      <c r="F234" s="3"/>
+    </row>
+    <row r="235" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B235" s="7">
+        <v>45829</v>
+      </c>
+      <c r="C235" s="3"/>
+      <c r="D235" s="3"/>
+      <c r="E235" s="3"/>
+      <c r="F235" s="3"/>
+    </row>
+    <row r="236" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B236" s="7">
+        <v>45830</v>
+      </c>
+      <c r="C236" s="3"/>
+      <c r="D236" s="3"/>
+      <c r="E236" s="3"/>
+      <c r="F236" s="3"/>
+    </row>
+    <row r="237" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B237" s="7">
+        <v>45831</v>
+      </c>
+      <c r="C237" s="3"/>
+      <c r="D237" s="3"/>
+      <c r="E237" s="3"/>
+      <c r="F237" s="3"/>
+    </row>
+    <row r="238" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G238" s="4">
+        <f>SUM(F231:F237)</f>
+        <v>11.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B208:F208"/>
     <mergeCell ref="B80:F80"/>
     <mergeCell ref="B229:F229"/>
@@ -3841,13 +3921,6 @@
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B223:F223"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B189:F189"/>
@@ -3857,13 +3930,6 @@
     <mergeCell ref="B153:F153"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B198:F198"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se terminó la seccion 3 para escritorio de la planta de tratamiento AR
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7379CE-4094-4ADC-A3BD-AC86282276C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4206E64-B0A7-4E49-88B5-992E8B216268}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -688,9 +688,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -698,6 +695,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -997,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="G239" sqref="G239"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="D232" sqref="D232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,13 +1031,13 @@
       <c r="J2" s="18"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
       <c r="J5" s="19" t="s">
         <v>7</v>
       </c>
@@ -1171,13 +1171,13 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1289,13 +1289,13 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1424,13 +1424,13 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
     </row>
     <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -1542,13 +1542,13 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
     </row>
     <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -1660,13 +1660,13 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
     </row>
     <row r="54" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -1778,13 +1778,13 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
     </row>
     <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -1896,13 +1896,13 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
     </row>
     <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -2014,13 +2014,13 @@
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
     </row>
     <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
@@ -2116,13 +2116,13 @@
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
     </row>
     <row r="90" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -2194,13 +2194,13 @@
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="12" t="s">
+      <c r="B98" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
     </row>
     <row r="99" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -2280,13 +2280,13 @@
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="12" t="s">
+      <c r="B107" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
     </row>
     <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -2382,13 +2382,13 @@
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="12" t="s">
+      <c r="B116" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
+      <c r="C116" s="15"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
     </row>
     <row r="117" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
@@ -2484,13 +2484,13 @@
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="12" t="s">
+      <c r="B125" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C125" s="12"/>
-      <c r="D125" s="12"/>
-      <c r="E125" s="12"/>
-      <c r="F125" s="12"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
     </row>
     <row r="126" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
@@ -2588,13 +2588,13 @@
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="12" t="s">
+      <c r="B134" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C134" s="12"/>
-      <c r="D134" s="12"/>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12"/>
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
     </row>
     <row r="135" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
@@ -2690,13 +2690,13 @@
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="12" t="s">
+      <c r="B143" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C143" s="12"/>
-      <c r="D143" s="12"/>
-      <c r="E143" s="12"/>
-      <c r="F143" s="12"/>
+      <c r="C143" s="15"/>
+      <c r="D143" s="15"/>
+      <c r="E143" s="15"/>
+      <c r="F143" s="15"/>
     </row>
     <row r="144" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
@@ -2817,13 +2817,13 @@
       <c r="N152"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B153" s="12" t="s">
+      <c r="B153" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C153" s="12"/>
-      <c r="D153" s="12"/>
-      <c r="E153" s="12"/>
-      <c r="F153" s="12"/>
+      <c r="C153" s="15"/>
+      <c r="D153" s="15"/>
+      <c r="E153" s="15"/>
+      <c r="F153" s="15"/>
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153"/>
@@ -2937,13 +2937,13 @@
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B162" s="12" t="s">
+      <c r="B162" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C162" s="12"/>
-      <c r="D162" s="12"/>
-      <c r="E162" s="12"/>
-      <c r="F162" s="12"/>
+      <c r="C162" s="15"/>
+      <c r="D162" s="15"/>
+      <c r="E162" s="15"/>
+      <c r="F162" s="15"/>
     </row>
     <row r="163" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
@@ -3072,13 +3072,13 @@
       </c>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B172" s="12" t="s">
+      <c r="B172" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C172" s="12"/>
-      <c r="D172" s="12"/>
-      <c r="E172" s="12"/>
-      <c r="F172" s="12"/>
+      <c r="C172" s="15"/>
+      <c r="D172" s="15"/>
+      <c r="E172" s="15"/>
+      <c r="F172" s="15"/>
     </row>
     <row r="173" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
@@ -3184,13 +3184,13 @@
       <c r="F179"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B180" s="12" t="s">
+      <c r="B180" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C180" s="12"/>
-      <c r="D180" s="12"/>
-      <c r="E180" s="12"/>
-      <c r="F180" s="12"/>
+      <c r="C180" s="15"/>
+      <c r="D180" s="15"/>
+      <c r="E180" s="15"/>
+      <c r="F180" s="15"/>
     </row>
     <row r="181" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
@@ -3310,13 +3310,13 @@
       <c r="D188" s="1"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="12" t="s">
+      <c r="B189" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C189" s="12"/>
-      <c r="D189" s="12"/>
-      <c r="E189" s="12"/>
-      <c r="F189" s="12"/>
+      <c r="C189" s="15"/>
+      <c r="D189" s="15"/>
+      <c r="E189" s="15"/>
+      <c r="F189" s="15"/>
     </row>
     <row r="190" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
@@ -3415,13 +3415,13 @@
       </c>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B198" s="12" t="s">
+      <c r="B198" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C198" s="12"/>
-      <c r="D198" s="12"/>
-      <c r="E198" s="12"/>
-      <c r="F198" s="12"/>
+      <c r="C198" s="15"/>
+      <c r="D198" s="15"/>
+      <c r="E198" s="15"/>
+      <c r="F198" s="15"/>
     </row>
     <row r="199" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
@@ -3552,13 +3552,13 @@
       </c>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B208" s="12" t="s">
+      <c r="B208" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C208" s="12"/>
-      <c r="D208" s="12"/>
-      <c r="E208" s="12"/>
-      <c r="F208" s="12"/>
+      <c r="C208" s="15"/>
+      <c r="D208" s="15"/>
+      <c r="E208" s="15"/>
+      <c r="F208" s="15"/>
     </row>
     <row r="209" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
@@ -3606,13 +3606,13 @@
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B213" s="13" t="s">
+      <c r="B213" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C213" s="14"/>
-      <c r="D213" s="14"/>
-      <c r="E213" s="14"/>
-      <c r="F213" s="15"/>
+      <c r="C213" s="13"/>
+      <c r="D213" s="13"/>
+      <c r="E213" s="13"/>
+      <c r="F213" s="14"/>
     </row>
     <row r="214" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B214" s="2" t="s">
@@ -3670,13 +3670,13 @@
       </c>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B218" s="13" t="s">
+      <c r="B218" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C218" s="14"/>
-      <c r="D218" s="14"/>
-      <c r="E218" s="14"/>
-      <c r="F218" s="15"/>
+      <c r="C218" s="13"/>
+      <c r="D218" s="13"/>
+      <c r="E218" s="13"/>
+      <c r="F218" s="14"/>
     </row>
     <row r="219" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B219" s="2" t="s">
@@ -3734,13 +3734,13 @@
       </c>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B223" s="13" t="s">
+      <c r="B223" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="C223" s="14"/>
-      <c r="D223" s="14"/>
-      <c r="E223" s="14"/>
-      <c r="F223" s="15"/>
+      <c r="C223" s="13"/>
+      <c r="D223" s="13"/>
+      <c r="E223" s="13"/>
+      <c r="F223" s="14"/>
     </row>
     <row r="224" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B224" s="2" t="s">
@@ -3788,13 +3788,13 @@
       </c>
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B229" s="13" t="s">
+      <c r="B229" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C229" s="14"/>
-      <c r="D229" s="14"/>
-      <c r="E229" s="14"/>
-      <c r="F229" s="15"/>
+      <c r="C229" s="13"/>
+      <c r="D229" s="13"/>
+      <c r="E229" s="13"/>
+      <c r="F229" s="14"/>
     </row>
     <row r="230" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B230" s="2" t="s">
@@ -3900,21 +3900,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B208:F208"/>
     <mergeCell ref="B80:F80"/>
     <mergeCell ref="B229:F229"/>
     <mergeCell ref="B44:F44"/>
@@ -3930,6 +3915,21 @@
     <mergeCell ref="B153:F153"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B208:F208"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se terminó la tercer parte y se llego hasta la animasión de la cuarta en pantallas de escritorio
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4206E64-B0A7-4E49-88B5-992E8B216268}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23BCCB6-5089-482A-ACF9-B0AD45EDBE17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="160">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -497,6 +497,15 @@
   </si>
   <si>
     <t>8:00 -12:00, 18:00 -21:00</t>
+  </si>
+  <si>
+    <t>Se terminó la tercer parte y se avanzó hasta la animasión de la cuarta</t>
+  </si>
+  <si>
+    <t>Se terminó la tercer parte y se llego hasta la animasión de la cuarta en pantallas de escritorio</t>
+  </si>
+  <si>
+    <t>10:30-13:00, 15:00-19:30</t>
   </si>
 </sst>
 </file>
@@ -688,6 +697,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -695,9 +707,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -998,7 +1007,7 @@
   <dimension ref="B1:N238"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="D232" sqref="D232"/>
+      <selection activeCell="F234" sqref="F234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1025,7 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45826</v>
+        <v>45827</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
@@ -1031,13 +1040,13 @@
       <c r="J2" s="18"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
       <c r="J5" s="19" t="s">
         <v>7</v>
       </c>
@@ -1061,7 +1070,7 @@
       </c>
       <c r="J6" s="20">
         <f>SUM(G12:G1202)</f>
-        <v>311.2</v>
+        <v>318.2</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1118,7 +1127,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>168.8</v>
+        <v>161.80000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1139,7 +1148,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>42.2</v>
+        <v>40.450000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1160,7 +1169,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>1.0550000000000002</v>
+        <v>1.01125</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -1171,13 +1180,13 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1289,13 +1298,13 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1424,13 +1433,13 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -1542,13 +1551,13 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
     </row>
     <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -1660,13 +1669,13 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
     </row>
     <row r="54" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -1778,13 +1787,13 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
     </row>
     <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -1896,13 +1905,13 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="15"/>
-      <c r="F71" s="15"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
     </row>
     <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -2014,13 +2023,13 @@
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
     </row>
     <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
@@ -2116,13 +2125,13 @@
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="15"/>
-      <c r="F89" s="15"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
     </row>
     <row r="90" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -2194,13 +2203,13 @@
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="15" t="s">
+      <c r="B98" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="15"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="15"/>
-      <c r="F98" s="15"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
     </row>
     <row r="99" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -2280,13 +2289,13 @@
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="15"/>
-      <c r="F107" s="15"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12"/>
     </row>
     <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -2382,13 +2391,13 @@
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="15" t="s">
+      <c r="B116" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="15"/>
-      <c r="E116" s="15"/>
-      <c r="F116" s="15"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
     </row>
     <row r="117" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
@@ -2484,13 +2493,13 @@
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="15" t="s">
+      <c r="B125" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="15"/>
-      <c r="F125" s="15"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
     </row>
     <row r="126" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
@@ -2588,13 +2597,13 @@
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="15" t="s">
+      <c r="B134" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C134" s="15"/>
-      <c r="D134" s="15"/>
-      <c r="E134" s="15"/>
-      <c r="F134" s="15"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
     </row>
     <row r="135" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
@@ -2690,13 +2699,13 @@
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="15" t="s">
+      <c r="B143" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C143" s="15"/>
-      <c r="D143" s="15"/>
-      <c r="E143" s="15"/>
-      <c r="F143" s="15"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="12"/>
     </row>
     <row r="144" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
@@ -2817,13 +2826,13 @@
       <c r="N152"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B153" s="15" t="s">
+      <c r="B153" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C153" s="15"/>
-      <c r="D153" s="15"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
+      <c r="C153" s="12"/>
+      <c r="D153" s="12"/>
+      <c r="E153" s="12"/>
+      <c r="F153" s="12"/>
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153"/>
@@ -2937,13 +2946,13 @@
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B162" s="15" t="s">
+      <c r="B162" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C162" s="15"/>
-      <c r="D162" s="15"/>
-      <c r="E162" s="15"/>
-      <c r="F162" s="15"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="12"/>
+      <c r="E162" s="12"/>
+      <c r="F162" s="12"/>
     </row>
     <row r="163" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
@@ -3072,13 +3081,13 @@
       </c>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B172" s="15" t="s">
+      <c r="B172" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C172" s="15"/>
-      <c r="D172" s="15"/>
-      <c r="E172" s="15"/>
-      <c r="F172" s="15"/>
+      <c r="C172" s="12"/>
+      <c r="D172" s="12"/>
+      <c r="E172" s="12"/>
+      <c r="F172" s="12"/>
     </row>
     <row r="173" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
@@ -3184,13 +3193,13 @@
       <c r="F179"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B180" s="15" t="s">
+      <c r="B180" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C180" s="15"/>
-      <c r="D180" s="15"/>
-      <c r="E180" s="15"/>
-      <c r="F180" s="15"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="12"/>
+      <c r="F180" s="12"/>
     </row>
     <row r="181" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
@@ -3310,13 +3319,13 @@
       <c r="D188" s="1"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="15" t="s">
+      <c r="B189" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C189" s="15"/>
-      <c r="D189" s="15"/>
-      <c r="E189" s="15"/>
-      <c r="F189" s="15"/>
+      <c r="C189" s="12"/>
+      <c r="D189" s="12"/>
+      <c r="E189" s="12"/>
+      <c r="F189" s="12"/>
     </row>
     <row r="190" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
@@ -3415,13 +3424,13 @@
       </c>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B198" s="15" t="s">
+      <c r="B198" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C198" s="15"/>
-      <c r="D198" s="15"/>
-      <c r="E198" s="15"/>
-      <c r="F198" s="15"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="12"/>
+      <c r="E198" s="12"/>
+      <c r="F198" s="12"/>
     </row>
     <row r="199" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
@@ -3552,13 +3561,13 @@
       </c>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B208" s="15" t="s">
+      <c r="B208" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C208" s="15"/>
-      <c r="D208" s="15"/>
-      <c r="E208" s="15"/>
-      <c r="F208" s="15"/>
+      <c r="C208" s="12"/>
+      <c r="D208" s="12"/>
+      <c r="E208" s="12"/>
+      <c r="F208" s="12"/>
     </row>
     <row r="209" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
@@ -3606,13 +3615,13 @@
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B213" s="12" t="s">
+      <c r="B213" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C213" s="13"/>
-      <c r="D213" s="13"/>
-      <c r="E213" s="13"/>
-      <c r="F213" s="14"/>
+      <c r="C213" s="14"/>
+      <c r="D213" s="14"/>
+      <c r="E213" s="14"/>
+      <c r="F213" s="15"/>
     </row>
     <row r="214" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B214" s="2" t="s">
@@ -3670,13 +3679,13 @@
       </c>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B218" s="12" t="s">
+      <c r="B218" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C218" s="13"/>
-      <c r="D218" s="13"/>
-      <c r="E218" s="13"/>
-      <c r="F218" s="14"/>
+      <c r="C218" s="14"/>
+      <c r="D218" s="14"/>
+      <c r="E218" s="14"/>
+      <c r="F218" s="15"/>
     </row>
     <row r="219" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B219" s="2" t="s">
@@ -3734,13 +3743,13 @@
       </c>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B223" s="12" t="s">
+      <c r="B223" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C223" s="13"/>
-      <c r="D223" s="13"/>
-      <c r="E223" s="13"/>
-      <c r="F223" s="14"/>
+      <c r="C223" s="14"/>
+      <c r="D223" s="14"/>
+      <c r="E223" s="14"/>
+      <c r="F223" s="15"/>
     </row>
     <row r="224" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B224" s="2" t="s">
@@ -3788,13 +3797,13 @@
       </c>
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B229" s="12" t="s">
+      <c r="B229" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="C229" s="13"/>
-      <c r="D229" s="13"/>
-      <c r="E229" s="13"/>
-      <c r="F229" s="14"/>
+      <c r="C229" s="14"/>
+      <c r="D229" s="14"/>
+      <c r="E229" s="14"/>
+      <c r="F229" s="15"/>
     </row>
     <row r="230" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B230" s="2" t="s">
@@ -3847,14 +3856,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B233" s="7">
         <v>45827</v>
       </c>
-      <c r="C233" s="3"/>
-      <c r="D233" s="3"/>
-      <c r="E233" s="3"/>
-      <c r="F233" s="3"/>
+      <c r="C233" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F233" s="3">
+        <v>7</v>
+      </c>
     </row>
     <row r="234" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B234" s="7">
@@ -3895,11 +3912,25 @@
     <row r="238" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G238" s="4">
         <f>SUM(F231:F237)</f>
-        <v>11.5</v>
+        <v>18.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B80:F80"/>
     <mergeCell ref="B229:F229"/>
     <mergeCell ref="B44:F44"/>
@@ -3915,21 +3946,7 @@
     <mergeCell ref="B153:F153"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B208:F208"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se ha terminado la cuarta sección y la quinta, solo falta animarla. Esto para la pantalla en escritorio
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23BCCB6-5089-482A-ACF9-B0AD45EDBE17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015F9ACC-DA11-467F-8EC2-DF428E70003F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="166">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -506,6 +506,24 @@
   </si>
   <si>
     <t>10:30-13:00, 15:00-19:30</t>
+  </si>
+  <si>
+    <t>Se terminó la animación y se avanzo hata el final de la quinta sección en escritorio</t>
+  </si>
+  <si>
+    <t>Se ha terminado la cuarta sección y la quinta, solo falta animarla. Esto para la pantalla en escritorio</t>
+  </si>
+  <si>
+    <t>8:00-12:00, 18:00-21:00</t>
+  </si>
+  <si>
+    <t>Se terminarón las animaciones en la quinta seccion</t>
+  </si>
+  <si>
+    <t>Se terminarón las animaciones en la quinta sección</t>
+  </si>
+  <si>
+    <t>19:00-22:30</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="F234" sqref="F234"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="D235" sqref="D235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1043,7 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45827</v>
+        <v>45833</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
@@ -1070,7 +1088,7 @@
       </c>
       <c r="J6" s="20">
         <f>SUM(G12:G1202)</f>
-        <v>318.2</v>
+        <v>328.7</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1127,7 +1145,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>161.80000000000001</v>
+        <v>151.30000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1148,7 +1166,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>40.450000000000003</v>
+        <v>37.825000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1169,7 +1187,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>1.01125</v>
+        <v>0.94562500000000005</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -3877,19 +3895,33 @@
       <c r="B234" s="7">
         <v>45828</v>
       </c>
-      <c r="C234" s="3"/>
-      <c r="D234" s="3"/>
-      <c r="E234" s="3"/>
+      <c r="C234" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="F234" s="3"/>
     </row>
-    <row r="235" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B235" s="7">
         <v>45829</v>
       </c>
-      <c r="C235" s="3"/>
-      <c r="D235" s="3"/>
-      <c r="E235" s="3"/>
-      <c r="F235" s="3"/>
+      <c r="C235" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F235" s="3">
+        <v>7</v>
+      </c>
     </row>
     <row r="236" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B236" s="7">
@@ -3900,19 +3932,27 @@
       <c r="E236" s="3"/>
       <c r="F236" s="3"/>
     </row>
-    <row r="237" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B237" s="7">
         <v>45831</v>
       </c>
-      <c r="C237" s="3"/>
-      <c r="D237" s="3"/>
-      <c r="E237" s="3"/>
-      <c r="F237" s="3"/>
+      <c r="C237" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F237" s="3">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="238" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G238" s="4">
         <f>SUM(F231:F237)</f>
-        <v>18.5</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se empezarón las funcionalidades para los videos, para pantallas de escritorio en la planta de tratamiento AR
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015F9ACC-DA11-467F-8EC2-DF428E70003F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E36D370-EC5C-4F08-9C79-F32E363DB3A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="169">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -524,6 +524,15 @@
   </si>
   <si>
     <t>19:00-22:30</t>
+  </si>
+  <si>
+    <t>Se empezarón las funcionalidades para los videos en la página</t>
+  </si>
+  <si>
+    <t>Se empezarón las funcionalidades para los videos, para pantallas de escritorio en la planta de tratamiento AR</t>
+  </si>
+  <si>
+    <t>8:00-10:00, 17:30-19:30</t>
   </si>
 </sst>
 </file>
@@ -715,9 +724,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -725,6 +731,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1022,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N238"/>
+  <dimension ref="B1:N250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="D235" sqref="D235"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="D243" sqref="D243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,13 +1067,13 @@
       <c r="J2" s="18"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
       <c r="J5" s="19" t="s">
         <v>7</v>
       </c>
@@ -1088,7 +1097,7 @@
       </c>
       <c r="J6" s="20">
         <f>SUM(G12:G1202)</f>
-        <v>328.7</v>
+        <v>332.7</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1145,7 +1154,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>151.30000000000001</v>
+        <v>147.30000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1166,7 +1175,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>37.825000000000003</v>
+        <v>36.825000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1187,7 +1196,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>0.94562500000000005</v>
+        <v>0.92062500000000003</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -1198,13 +1207,13 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1316,13 +1325,13 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1451,13 +1460,13 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
     </row>
     <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -1569,13 +1578,13 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
     </row>
     <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -1687,13 +1696,13 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
     </row>
     <row r="54" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -1805,13 +1814,13 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
     </row>
     <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -1923,13 +1932,13 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
     </row>
     <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -2041,13 +2050,13 @@
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
     </row>
     <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
@@ -2143,13 +2152,13 @@
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
     </row>
     <row r="90" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -2221,13 +2230,13 @@
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="12" t="s">
+      <c r="B98" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
     </row>
     <row r="99" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -2307,13 +2316,13 @@
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="12" t="s">
+      <c r="B107" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
     </row>
     <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -2409,13 +2418,13 @@
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="12" t="s">
+      <c r="B116" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
+      <c r="C116" s="15"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
     </row>
     <row r="117" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
@@ -2511,13 +2520,13 @@
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="12" t="s">
+      <c r="B125" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C125" s="12"/>
-      <c r="D125" s="12"/>
-      <c r="E125" s="12"/>
-      <c r="F125" s="12"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
     </row>
     <row r="126" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
@@ -2615,13 +2624,13 @@
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="12" t="s">
+      <c r="B134" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C134" s="12"/>
-      <c r="D134" s="12"/>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12"/>
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
     </row>
     <row r="135" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
@@ -2717,13 +2726,13 @@
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="12" t="s">
+      <c r="B143" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C143" s="12"/>
-      <c r="D143" s="12"/>
-      <c r="E143" s="12"/>
-      <c r="F143" s="12"/>
+      <c r="C143" s="15"/>
+      <c r="D143" s="15"/>
+      <c r="E143" s="15"/>
+      <c r="F143" s="15"/>
     </row>
     <row r="144" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
@@ -2844,13 +2853,13 @@
       <c r="N152"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B153" s="12" t="s">
+      <c r="B153" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C153" s="12"/>
-      <c r="D153" s="12"/>
-      <c r="E153" s="12"/>
-      <c r="F153" s="12"/>
+      <c r="C153" s="15"/>
+      <c r="D153" s="15"/>
+      <c r="E153" s="15"/>
+      <c r="F153" s="15"/>
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153"/>
@@ -2964,13 +2973,13 @@
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B162" s="12" t="s">
+      <c r="B162" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C162" s="12"/>
-      <c r="D162" s="12"/>
-      <c r="E162" s="12"/>
-      <c r="F162" s="12"/>
+      <c r="C162" s="15"/>
+      <c r="D162" s="15"/>
+      <c r="E162" s="15"/>
+      <c r="F162" s="15"/>
     </row>
     <row r="163" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
@@ -3099,13 +3108,13 @@
       </c>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B172" s="12" t="s">
+      <c r="B172" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C172" s="12"/>
-      <c r="D172" s="12"/>
-      <c r="E172" s="12"/>
-      <c r="F172" s="12"/>
+      <c r="C172" s="15"/>
+      <c r="D172" s="15"/>
+      <c r="E172" s="15"/>
+      <c r="F172" s="15"/>
     </row>
     <row r="173" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
@@ -3211,13 +3220,13 @@
       <c r="F179"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B180" s="12" t="s">
+      <c r="B180" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C180" s="12"/>
-      <c r="D180" s="12"/>
-      <c r="E180" s="12"/>
-      <c r="F180" s="12"/>
+      <c r="C180" s="15"/>
+      <c r="D180" s="15"/>
+      <c r="E180" s="15"/>
+      <c r="F180" s="15"/>
     </row>
     <row r="181" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
@@ -3337,13 +3346,13 @@
       <c r="D188" s="1"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="12" t="s">
+      <c r="B189" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C189" s="12"/>
-      <c r="D189" s="12"/>
-      <c r="E189" s="12"/>
-      <c r="F189" s="12"/>
+      <c r="C189" s="15"/>
+      <c r="D189" s="15"/>
+      <c r="E189" s="15"/>
+      <c r="F189" s="15"/>
     </row>
     <row r="190" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
@@ -3442,13 +3451,13 @@
       </c>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B198" s="12" t="s">
+      <c r="B198" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C198" s="12"/>
-      <c r="D198" s="12"/>
-      <c r="E198" s="12"/>
-      <c r="F198" s="12"/>
+      <c r="C198" s="15"/>
+      <c r="D198" s="15"/>
+      <c r="E198" s="15"/>
+      <c r="F198" s="15"/>
     </row>
     <row r="199" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
@@ -3579,13 +3588,13 @@
       </c>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B208" s="12" t="s">
+      <c r="B208" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C208" s="12"/>
-      <c r="D208" s="12"/>
-      <c r="E208" s="12"/>
-      <c r="F208" s="12"/>
+      <c r="C208" s="15"/>
+      <c r="D208" s="15"/>
+      <c r="E208" s="15"/>
+      <c r="F208" s="15"/>
     </row>
     <row r="209" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
@@ -3633,13 +3642,13 @@
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B213" s="13" t="s">
+      <c r="B213" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C213" s="14"/>
-      <c r="D213" s="14"/>
-      <c r="E213" s="14"/>
-      <c r="F213" s="15"/>
+      <c r="C213" s="13"/>
+      <c r="D213" s="13"/>
+      <c r="E213" s="13"/>
+      <c r="F213" s="14"/>
     </row>
     <row r="214" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B214" s="2" t="s">
@@ -3697,13 +3706,13 @@
       </c>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B218" s="13" t="s">
+      <c r="B218" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C218" s="14"/>
-      <c r="D218" s="14"/>
-      <c r="E218" s="14"/>
-      <c r="F218" s="15"/>
+      <c r="C218" s="13"/>
+      <c r="D218" s="13"/>
+      <c r="E218" s="13"/>
+      <c r="F218" s="14"/>
     </row>
     <row r="219" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B219" s="2" t="s">
@@ -3761,13 +3770,13 @@
       </c>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B223" s="13" t="s">
+      <c r="B223" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="C223" s="14"/>
-      <c r="D223" s="14"/>
-      <c r="E223" s="14"/>
-      <c r="F223" s="15"/>
+      <c r="C223" s="13"/>
+      <c r="D223" s="13"/>
+      <c r="E223" s="13"/>
+      <c r="F223" s="14"/>
     </row>
     <row r="224" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B224" s="2" t="s">
@@ -3815,13 +3824,13 @@
       </c>
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B229" s="13" t="s">
+      <c r="B229" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C229" s="14"/>
-      <c r="D229" s="14"/>
-      <c r="E229" s="14"/>
-      <c r="F229" s="15"/>
+      <c r="C229" s="13"/>
+      <c r="D229" s="13"/>
+      <c r="E229" s="13"/>
+      <c r="F229" s="14"/>
     </row>
     <row r="230" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B230" s="2" t="s">
@@ -3955,8 +3964,119 @@
         <v>29</v>
       </c>
     </row>
+    <row r="241" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B241" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C241" s="13"/>
+      <c r="D241" s="13"/>
+      <c r="E241" s="13"/>
+      <c r="F241" s="14"/>
+    </row>
+    <row r="242" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B242" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D242" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E242" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F242" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B243" s="7">
+        <v>45833</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F243" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B244" s="7">
+        <v>45834</v>
+      </c>
+      <c r="C244" s="3"/>
+      <c r="D244" s="3"/>
+      <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
+    </row>
+    <row r="245" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B245" s="7">
+        <v>45835</v>
+      </c>
+      <c r="C245" s="3"/>
+      <c r="D245" s="3"/>
+      <c r="E245" s="3"/>
+      <c r="F245" s="3"/>
+    </row>
+    <row r="246" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B246" s="7">
+        <v>45836</v>
+      </c>
+      <c r="C246" s="3"/>
+      <c r="D246" s="3"/>
+      <c r="E246" s="3"/>
+      <c r="F246" s="3"/>
+    </row>
+    <row r="247" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B247" s="7">
+        <v>45837</v>
+      </c>
+      <c r="C247" s="3"/>
+      <c r="D247" s="3"/>
+      <c r="E247" s="3"/>
+      <c r="F247" s="3"/>
+    </row>
+    <row r="248" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B248" s="7">
+        <v>45838</v>
+      </c>
+      <c r="C248" s="3"/>
+      <c r="D248" s="3"/>
+      <c r="E248" s="3"/>
+      <c r="F248" s="3"/>
+    </row>
+    <row r="249" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B249" s="7">
+        <v>45839</v>
+      </c>
+      <c r="C249" s="3"/>
+      <c r="D249" s="3"/>
+      <c r="E249" s="3"/>
+      <c r="F249" s="3"/>
+    </row>
+    <row r="250" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G250" s="4">
+        <f>SUM(F243:F249)</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="31">
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B213:F213"/>
     <mergeCell ref="B208:F208"/>
     <mergeCell ref="B198:F198"/>
@@ -3964,13 +4084,7 @@
     <mergeCell ref="B180:F180"/>
     <mergeCell ref="B172:F172"/>
     <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B241:F241"/>
     <mergeCell ref="B80:F80"/>
     <mergeCell ref="B229:F229"/>
     <mergeCell ref="B44:F44"/>
@@ -3986,7 +4100,6 @@
     <mergeCell ref="B153:F153"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B218:F218"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se terminarón las funcionalidades para los videos y se avanzaron responsivamente hasta la misma sección, para la planta de tratamiento AR
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E36D370-EC5C-4F08-9C79-F32E363DB3A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A33D55B-B746-4633-BAF6-F3A78B74DBF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="172">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -533,6 +533,15 @@
   </si>
   <si>
     <t>8:00-10:00, 17:30-19:30</t>
+  </si>
+  <si>
+    <t>Se terminarón las funcionalidades para los videos y se avanzaron responsivamente hasta la misma sección</t>
+  </si>
+  <si>
+    <t>Se terminarón las funcionalidades para los videos y se avanzaron responsivamente hasta la misma sección, para la planta de tratamiento AR</t>
+  </si>
+  <si>
+    <t>7:00-11:30, 14:30-19:00</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1043,7 @@
   <dimension ref="B1:N250"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="D243" sqref="D243"/>
+      <selection activeCell="G242" sqref="G242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1061,7 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45833</v>
+        <v>45834</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
@@ -1097,7 +1106,7 @@
       </c>
       <c r="J6" s="20">
         <f>SUM(G12:G1202)</f>
-        <v>332.7</v>
+        <v>341.7</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1154,7 +1163,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>147.30000000000001</v>
+        <v>138.30000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1175,7 +1184,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>36.825000000000003</v>
+        <v>34.575000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1196,7 +1205,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>0.92062500000000003</v>
+        <v>0.86437500000000012</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -4007,14 +4016,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B244" s="7">
         <v>45834</v>
       </c>
-      <c r="C244" s="3"/>
-      <c r="D244" s="3"/>
-      <c r="E244" s="3"/>
-      <c r="F244" s="3"/>
+      <c r="C244" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F244" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="245" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B245" s="7">
@@ -4064,26 +4081,11 @@
     <row r="250" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G250" s="4">
         <f>SUM(F243:F249)</f>
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B162:F162"/>
     <mergeCell ref="B241:F241"/>
     <mergeCell ref="B80:F80"/>
     <mergeCell ref="B229:F229"/>
@@ -4100,6 +4102,21 @@
     <mergeCell ref="B153:F153"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B162:F162"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se avanzo hasta el final de las funciones responsivas para la cuarta sección, para la planta de tratamiento AR
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A33D55B-B746-4633-BAF6-F3A78B74DBF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E30AC-1514-4B73-BDFB-4335756EE239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="175">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -542,6 +542,15 @@
   </si>
   <si>
     <t>7:00-11:30, 14:30-19:00</t>
+  </si>
+  <si>
+    <t>Se avanzo hasta el final de las funciones responsivas para la cuarta sección</t>
+  </si>
+  <si>
+    <t>Se avanzo hasta el final de las funciones responsivas para la cuarta sección, para la plata de tratamiento AR</t>
+  </si>
+  <si>
+    <t>7:00-11:00 - 18:00-21:30</t>
   </si>
 </sst>
 </file>
@@ -1040,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N250"/>
+  <dimension ref="B1:N248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="G242" sqref="G242"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="D245" sqref="D245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1070,7 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45834</v>
+        <v>45836</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
@@ -1105,8 +1114,8 @@
         <v>1</v>
       </c>
       <c r="J6" s="20">
-        <f>SUM(G12:G1202)</f>
-        <v>341.7</v>
+        <f>SUM(G12:G1200)</f>
+        <v>349.2</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1163,7 +1172,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>138.30000000000001</v>
+        <v>130.80000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1184,7 +1193,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>34.575000000000003</v>
+        <v>32.700000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1205,7 +1214,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>0.86437500000000012</v>
+        <v>0.81750000000000012</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -4033,14 +4042,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B245" s="7">
         <v>45835</v>
       </c>
-      <c r="C245" s="3"/>
-      <c r="D245" s="3"/>
-      <c r="E245" s="3"/>
-      <c r="F245" s="3"/>
+      <c r="C245" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E245" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F245" s="3">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="246" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B246" s="7">
@@ -4061,31 +4078,28 @@
       <c r="F247" s="3"/>
     </row>
     <row r="248" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B248" s="7">
-        <v>45838</v>
-      </c>
-      <c r="C248" s="3"/>
-      <c r="D248" s="3"/>
-      <c r="E248" s="3"/>
-      <c r="F248" s="3"/>
-    </row>
-    <row r="249" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B249" s="7">
-        <v>45839</v>
-      </c>
-      <c r="C249" s="3"/>
-      <c r="D249" s="3"/>
-      <c r="E249" s="3"/>
-      <c r="F249" s="3"/>
-    </row>
-    <row r="250" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G250" s="4">
-        <f>SUM(F243:F249)</f>
-        <v>13</v>
+      <c r="G248" s="4">
+        <f>SUM(F243:F247)</f>
+        <v>20.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B162:F162"/>
     <mergeCell ref="B241:F241"/>
     <mergeCell ref="B80:F80"/>
     <mergeCell ref="B229:F229"/>
@@ -4102,21 +4116,6 @@
     <mergeCell ref="B153:F153"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B162:F162"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se terminó la funcionalidad para la sección 4 y se empezaron a trabajar los cambios solicitados en la anterior reunión, para la planta de tratamiento AR
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E30AC-1514-4B73-BDFB-4335756EE239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E597A0F-D27D-4759-B17C-A1EF00F95BB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="178">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -547,10 +547,19 @@
     <t>Se avanzo hasta el final de las funciones responsivas para la cuarta sección</t>
   </si>
   <si>
-    <t>Se avanzo hasta el final de las funciones responsivas para la cuarta sección, para la plata de tratamiento AR</t>
-  </si>
-  <si>
     <t>7:00-11:00 - 18:00-21:30</t>
+  </si>
+  <si>
+    <t>Se terminó la funcionalidad para la sección 4 y se empezaron a trabajar los cambios solicitados en la anterior reunión</t>
+  </si>
+  <si>
+    <t>9:00 - 12:00, 13:30- 19:30</t>
+  </si>
+  <si>
+    <t>Se terminó la funcionalidad para la sección 4 y se empezaron a trabajar los cambios solicitados en la anterior reunión, para la planta de tratamiento AR</t>
+  </si>
+  <si>
+    <t>Se avanzo hasta el final de las funciones responsivas para la cuarta sección, para la planta de tratamiento AR</t>
   </si>
 </sst>
 </file>
@@ -1051,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="D245" sqref="D245"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="D246" sqref="D246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1124,7 @@
       </c>
       <c r="J6" s="20">
         <f>SUM(G12:G1200)</f>
-        <v>349.2</v>
+        <v>358.2</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1172,7 +1181,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>130.80000000000001</v>
+        <v>121.80000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1193,7 +1202,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>32.700000000000003</v>
+        <v>30.450000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1214,7 +1223,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>0.81750000000000012</v>
+        <v>0.76125000000000009</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -4050,23 +4059,31 @@
         <v>172</v>
       </c>
       <c r="D245" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E245" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="E245" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="F245" s="3">
         <v>7.5</v>
       </c>
     </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B246" s="7">
         <v>45836</v>
       </c>
-      <c r="C246" s="3"/>
-      <c r="D246" s="3"/>
-      <c r="E246" s="3"/>
-      <c r="F246" s="3"/>
+      <c r="C246" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E246" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F246" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="247" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B247" s="7">
@@ -4080,26 +4097,11 @@
     <row r="248" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G248" s="4">
         <f>SUM(F243:F247)</f>
-        <v>20.5</v>
+        <v>29.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B162:F162"/>
     <mergeCell ref="B241:F241"/>
     <mergeCell ref="B80:F80"/>
     <mergeCell ref="B229:F229"/>
@@ -4116,6 +4118,21 @@
     <mergeCell ref="B153:F153"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B162:F162"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se terminó una función para el control de GIFs de la sección 5, para la planta de tratamiento AR
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E597A0F-D27D-4759-B17C-A1EF00F95BB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD4F58B-C392-40F8-A9F7-D6CCCD539B5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOVIEMBRE 2024" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="191">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -560,6 +560,45 @@
   </si>
   <si>
     <t>Se avanzo hasta el final de las funciones responsivas para la cuarta sección, para la planta de tratamiento AR</t>
+  </si>
+  <si>
+    <t>Se realizarón los cambion responsivos para la sección 5</t>
+  </si>
+  <si>
+    <t>Se empezarón los cambios responsivos parara la sección 5</t>
+  </si>
+  <si>
+    <t>11:00-14:00</t>
+  </si>
+  <si>
+    <t>SEMANA 26</t>
+  </si>
+  <si>
+    <t>SEMANA 27</t>
+  </si>
+  <si>
+    <t>SEMANA 28</t>
+  </si>
+  <si>
+    <t>Se terminó la funcionalidad para la sección 5, se corrigierón detalles y se empezo a trabajar en la sección 6</t>
+  </si>
+  <si>
+    <t>Se terminó la funcionalidad para la sección 5, se corrigieron detalles y se empezo la sección 6, para la planta de tratamiento AR. Se presentarón problemas con los GIFs</t>
+  </si>
+  <si>
+    <t>7:00-11:30, 15:30-20:00</t>
+  </si>
+  <si>
+    <t>SEMANA 29</t>
+  </si>
+  <si>
+    <t>Se creó una función para el control del los GIFs, considerando su reinicio y optimización</t>
+  </si>
+  <si>
+    <t>Se terminó una función para el control de GIFs de la sección 5, para la planta de tratamiento AR</t>
+  </si>
+  <si>
+    <t>8:30-13:00, 15:30-20:00</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N248"/>
+  <dimension ref="B1:N264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
-      <selection activeCell="D246" sqref="D246"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="D271" sqref="D271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,7 +1118,7 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45836</v>
+        <v>45866</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
@@ -1123,8 +1162,8 @@
         <v>1</v>
       </c>
       <c r="J6" s="20">
-        <f>SUM(G12:G1200)</f>
-        <v>358.2</v>
+        <f>SUM(G12:G1193)</f>
+        <v>379.2</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1181,7 +1220,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>121.80000000000001</v>
+        <v>100.80000000000001</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1202,7 +1241,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>30.450000000000003</v>
+        <v>25.200000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1223,7 +1262,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>0.76125000000000009</v>
+        <v>0.63000000000000012</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -3993,7 +4032,7 @@
     </row>
     <row r="241" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B241" s="12" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="C241" s="13"/>
       <c r="D241" s="13"/>
@@ -4086,22 +4125,178 @@
       </c>
     </row>
     <row r="247" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B247" s="7">
-        <v>45837</v>
-      </c>
-      <c r="C247" s="3"/>
-      <c r="D247" s="3"/>
-      <c r="E247" s="3"/>
-      <c r="F247" s="3"/>
-    </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G248" s="4">
-        <f>SUM(F243:F247)</f>
+      <c r="G247" s="4">
+        <f>SUM(F243:F246)</f>
         <v>29.5</v>
       </c>
     </row>
+    <row r="249" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B249" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C249" s="13"/>
+      <c r="D249" s="13"/>
+      <c r="E249" s="13"/>
+      <c r="F249" s="14"/>
+    </row>
+    <row r="250" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B250" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F250" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B251" s="7">
+        <v>45841</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D251" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E251" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F251" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G252" s="4">
+        <f>SUM(F251:F251)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B255" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C255" s="13"/>
+      <c r="D255" s="13"/>
+      <c r="E255" s="13"/>
+      <c r="F255" s="14"/>
+    </row>
+    <row r="256" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B256" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D256" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E256" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F256" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B257" s="7">
+        <v>45862</v>
+      </c>
+      <c r="C257" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D257" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E257" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F257" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="258" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G258" s="4">
+        <f>SUM(F257:F257)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="261" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B261" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C261" s="13"/>
+      <c r="D261" s="13"/>
+      <c r="E261" s="13"/>
+      <c r="F261" s="14"/>
+    </row>
+    <row r="262" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B262" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D262" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E262" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F262" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B263" s="7">
+        <v>45866</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D263" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E263" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F263" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="264" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G264" s="4">
+        <f>SUM(F263:F263)</f>
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="34">
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B162:F162"/>
     <mergeCell ref="B241:F241"/>
     <mergeCell ref="B80:F80"/>
     <mergeCell ref="B229:F229"/>
@@ -4118,21 +4313,6 @@
     <mergeCell ref="B153:F153"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B162:F162"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se terminó la sección 5 en su forma resposiva y se solucionaron errores, para la planta de tratamiento AR
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD4F58B-C392-40F8-A9F7-D6CCCD539B5A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7D3AF3-81F6-4DB9-AA8A-C5C7C5278581}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="194">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -599,6 +599,15 @@
   </si>
   <si>
     <t>8:30-13:00, 15:30-20:00</t>
+  </si>
+  <si>
+    <t>Se terminó la sección 5 en su  forma responsiva</t>
+  </si>
+  <si>
+    <t>Se terminó l a sección 5 en su forma resposiva y se solucionaron errores, para la planta de tratamiento AR</t>
+  </si>
+  <si>
+    <t>6:00 - 11:00, 17:00 - 18:00</t>
   </si>
 </sst>
 </file>
@@ -1097,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N264"/>
+  <dimension ref="B1:N267"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="D271" sqref="D271"/>
+      <selection activeCell="F265" sqref="F265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1127,7 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45866</v>
+        <v>45869</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
@@ -1163,7 +1172,7 @@
       </c>
       <c r="J6" s="20">
         <f>SUM(G12:G1193)</f>
-        <v>379.2</v>
+        <v>385.2</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1220,7 +1229,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>100.80000000000001</v>
+        <v>94.800000000000011</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1241,7 +1250,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>25.200000000000003</v>
+        <v>23.700000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1262,7 +1271,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>0.63000000000000012</v>
+        <v>0.59250000000000003</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -4271,35 +4280,49 @@
         <v>9</v>
       </c>
     </row>
-    <row r="264" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G264" s="4">
-        <f>SUM(F263:F263)</f>
-        <v>9</v>
+    <row r="264" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B264" s="7">
+        <v>45869</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D264" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E264" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F264" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="265" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B265" s="7">
+        <v>45870</v>
+      </c>
+      <c r="C265" s="3"/>
+      <c r="D265" s="3"/>
+      <c r="E265" s="3"/>
+      <c r="F265" s="3"/>
+    </row>
+    <row r="266" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B266" s="7">
+        <v>45871</v>
+      </c>
+      <c r="C266" s="3"/>
+      <c r="D266" s="3"/>
+      <c r="E266" s="3"/>
+      <c r="F266" s="3"/>
+    </row>
+    <row r="267" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G267" s="4">
+        <f>SUM(F263:F266)</f>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B213:F213"/>
-    <mergeCell ref="B208:F208"/>
-    <mergeCell ref="B198:F198"/>
-    <mergeCell ref="B134:F134"/>
-    <mergeCell ref="B180:F180"/>
-    <mergeCell ref="B172:F172"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B229:F229"/>
     <mergeCell ref="B44:F44"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B62:F62"/>
@@ -4313,6 +4336,27 @@
     <mergeCell ref="B153:F153"/>
     <mergeCell ref="B143:F143"/>
     <mergeCell ref="B125:F125"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B213:F213"/>
+    <mergeCell ref="B208:F208"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B134:F134"/>
+    <mergeCell ref="B180:F180"/>
+    <mergeCell ref="B172:F172"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B229:F229"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se trabajo en los cambios solicitados en la última reunión, para la planta de tratamiento AR.
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7D3AF3-81F6-4DB9-AA8A-C5C7C5278581}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21E2189-57EE-4E11-8C3E-FEECC16F1975}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="203">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -608,6 +608,33 @@
   </si>
   <si>
     <t>6:00 - 11:00, 17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>SEMANA 30</t>
+  </si>
+  <si>
+    <t>Se agregarón efectos con observadores</t>
+  </si>
+  <si>
+    <t>8:00 - 13:00, 17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>Se trabajó actividades de la OGA</t>
+  </si>
+  <si>
+    <t>Se realizarón las actividades solicitadas de la OGA</t>
+  </si>
+  <si>
+    <t>10:00 - 13:00, 15:00 -18:00</t>
+  </si>
+  <si>
+    <t>Se trabajo en los cambios solicitados en la última reuinion</t>
+  </si>
+  <si>
+    <t>Se trabajo en los cambios solicitados en la última reunión, para la planta de tratamiento AR.</t>
+  </si>
+  <si>
+    <t>8:00 -12:00, 15:00 - 18:00</t>
   </si>
 </sst>
 </file>
@@ -799,15 +826,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -824,6 +842,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1106,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N267"/>
+  <dimension ref="B1:N275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="F265" sqref="F265"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="D273" sqref="D273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,32 +1154,32 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45869</v>
+        <v>45876</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="J5" s="19" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="J5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="19"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1170,11 +1197,11 @@
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="20">
-        <f>SUM(G12:G1193)</f>
-        <v>385.2</v>
-      </c>
-      <c r="K6" s="20"/>
+      <c r="J6" s="17">
+        <f>SUM(G12:G1191)</f>
+        <v>404.2</v>
+      </c>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
@@ -1229,7 +1256,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>94.800000000000011</v>
+        <v>75.800000000000011</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1250,7 +1277,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>23.700000000000003</v>
+        <v>18.950000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1271,7 +1298,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>0.59250000000000003</v>
+        <v>0.47375000000000006</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -1282,13 +1309,13 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1400,13 +1427,13 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1535,13 +1562,13 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -1653,13 +1680,13 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
     </row>
     <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -1771,13 +1798,13 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
     </row>
     <row r="54" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -1889,13 +1916,13 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
     </row>
     <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -2007,13 +2034,13 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="15" t="s">
+      <c r="B71" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="15"/>
-      <c r="F71" s="15"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
     </row>
     <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -2125,13 +2152,13 @@
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
     </row>
     <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
@@ -2227,13 +2254,13 @@
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="15"/>
-      <c r="F89" s="15"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
     </row>
     <row r="90" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -2305,13 +2332,13 @@
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="15" t="s">
+      <c r="B98" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="15"/>
-      <c r="D98" s="15"/>
-      <c r="E98" s="15"/>
-      <c r="F98" s="15"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
     </row>
     <row r="99" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -2391,13 +2418,13 @@
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="15"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="15"/>
-      <c r="F107" s="15"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12"/>
     </row>
     <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -2493,13 +2520,13 @@
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="15" t="s">
+      <c r="B116" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C116" s="15"/>
-      <c r="D116" s="15"/>
-      <c r="E116" s="15"/>
-      <c r="F116" s="15"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12"/>
     </row>
     <row r="117" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
@@ -2595,13 +2622,13 @@
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="15" t="s">
+      <c r="B125" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15"/>
-      <c r="E125" s="15"/>
-      <c r="F125" s="15"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
     </row>
     <row r="126" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
@@ -2699,13 +2726,13 @@
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="15" t="s">
+      <c r="B134" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C134" s="15"/>
-      <c r="D134" s="15"/>
-      <c r="E134" s="15"/>
-      <c r="F134" s="15"/>
+      <c r="C134" s="12"/>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
     </row>
     <row r="135" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
@@ -2801,13 +2828,13 @@
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="15" t="s">
+      <c r="B143" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C143" s="15"/>
-      <c r="D143" s="15"/>
-      <c r="E143" s="15"/>
-      <c r="F143" s="15"/>
+      <c r="C143" s="12"/>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="12"/>
     </row>
     <row r="144" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
@@ -2928,13 +2955,13 @@
       <c r="N152"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B153" s="15" t="s">
+      <c r="B153" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C153" s="15"/>
-      <c r="D153" s="15"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="15"/>
+      <c r="C153" s="12"/>
+      <c r="D153" s="12"/>
+      <c r="E153" s="12"/>
+      <c r="F153" s="12"/>
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153"/>
@@ -3048,13 +3075,13 @@
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B162" s="15" t="s">
+      <c r="B162" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C162" s="15"/>
-      <c r="D162" s="15"/>
-      <c r="E162" s="15"/>
-      <c r="F162" s="15"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="12"/>
+      <c r="E162" s="12"/>
+      <c r="F162" s="12"/>
     </row>
     <row r="163" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
@@ -3183,13 +3210,13 @@
       </c>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B172" s="15" t="s">
+      <c r="B172" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C172" s="15"/>
-      <c r="D172" s="15"/>
-      <c r="E172" s="15"/>
-      <c r="F172" s="15"/>
+      <c r="C172" s="12"/>
+      <c r="D172" s="12"/>
+      <c r="E172" s="12"/>
+      <c r="F172" s="12"/>
     </row>
     <row r="173" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
@@ -3295,13 +3322,13 @@
       <c r="F179"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B180" s="15" t="s">
+      <c r="B180" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C180" s="15"/>
-      <c r="D180" s="15"/>
-      <c r="E180" s="15"/>
-      <c r="F180" s="15"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="12"/>
+      <c r="F180" s="12"/>
     </row>
     <row r="181" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
@@ -3421,13 +3448,13 @@
       <c r="D188" s="1"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="15" t="s">
+      <c r="B189" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C189" s="15"/>
-      <c r="D189" s="15"/>
-      <c r="E189" s="15"/>
-      <c r="F189" s="15"/>
+      <c r="C189" s="12"/>
+      <c r="D189" s="12"/>
+      <c r="E189" s="12"/>
+      <c r="F189" s="12"/>
     </row>
     <row r="190" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
@@ -3526,13 +3553,13 @@
       </c>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B198" s="15" t="s">
+      <c r="B198" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="C198" s="15"/>
-      <c r="D198" s="15"/>
-      <c r="E198" s="15"/>
-      <c r="F198" s="15"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="12"/>
+      <c r="E198" s="12"/>
+      <c r="F198" s="12"/>
     </row>
     <row r="199" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
@@ -3663,13 +3690,13 @@
       </c>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B208" s="15" t="s">
+      <c r="B208" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C208" s="15"/>
-      <c r="D208" s="15"/>
-      <c r="E208" s="15"/>
-      <c r="F208" s="15"/>
+      <c r="C208" s="12"/>
+      <c r="D208" s="12"/>
+      <c r="E208" s="12"/>
+      <c r="F208" s="12"/>
     </row>
     <row r="209" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
@@ -3717,13 +3744,13 @@
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B213" s="12" t="s">
+      <c r="B213" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="C213" s="13"/>
-      <c r="D213" s="13"/>
-      <c r="E213" s="13"/>
-      <c r="F213" s="14"/>
+      <c r="C213" s="19"/>
+      <c r="D213" s="19"/>
+      <c r="E213" s="19"/>
+      <c r="F213" s="20"/>
     </row>
     <row r="214" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B214" s="2" t="s">
@@ -3781,13 +3808,13 @@
       </c>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B218" s="12" t="s">
+      <c r="B218" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C218" s="13"/>
-      <c r="D218" s="13"/>
-      <c r="E218" s="13"/>
-      <c r="F218" s="14"/>
+      <c r="C218" s="19"/>
+      <c r="D218" s="19"/>
+      <c r="E218" s="19"/>
+      <c r="F218" s="20"/>
     </row>
     <row r="219" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B219" s="2" t="s">
@@ -3845,13 +3872,13 @@
       </c>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B223" s="12" t="s">
+      <c r="B223" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C223" s="13"/>
-      <c r="D223" s="13"/>
-      <c r="E223" s="13"/>
-      <c r="F223" s="14"/>
+      <c r="C223" s="19"/>
+      <c r="D223" s="19"/>
+      <c r="E223" s="19"/>
+      <c r="F223" s="20"/>
     </row>
     <row r="224" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B224" s="2" t="s">
@@ -3899,13 +3926,13 @@
       </c>
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B229" s="12" t="s">
+      <c r="B229" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="C229" s="13"/>
-      <c r="D229" s="13"/>
-      <c r="E229" s="13"/>
-      <c r="F229" s="14"/>
+      <c r="C229" s="19"/>
+      <c r="D229" s="19"/>
+      <c r="E229" s="19"/>
+      <c r="F229" s="20"/>
     </row>
     <row r="230" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B230" s="2" t="s">
@@ -4040,13 +4067,13 @@
       </c>
     </row>
     <row r="241" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B241" s="12" t="s">
+      <c r="B241" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C241" s="13"/>
-      <c r="D241" s="13"/>
-      <c r="E241" s="13"/>
-      <c r="F241" s="14"/>
+      <c r="C241" s="19"/>
+      <c r="D241" s="19"/>
+      <c r="E241" s="19"/>
+      <c r="F241" s="20"/>
     </row>
     <row r="242" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B242" s="2" t="s">
@@ -4140,13 +4167,13 @@
       </c>
     </row>
     <row r="249" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B249" s="12" t="s">
+      <c r="B249" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="C249" s="13"/>
-      <c r="D249" s="13"/>
-      <c r="E249" s="13"/>
-      <c r="F249" s="14"/>
+      <c r="C249" s="19"/>
+      <c r="D249" s="19"/>
+      <c r="E249" s="19"/>
+      <c r="F249" s="20"/>
     </row>
     <row r="250" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B250" s="2" t="s">
@@ -4189,13 +4216,13 @@
       </c>
     </row>
     <row r="255" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B255" s="12" t="s">
+      <c r="B255" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="C255" s="13"/>
-      <c r="D255" s="13"/>
-      <c r="E255" s="13"/>
-      <c r="F255" s="14"/>
+      <c r="C255" s="19"/>
+      <c r="D255" s="19"/>
+      <c r="E255" s="19"/>
+      <c r="F255" s="20"/>
     </row>
     <row r="256" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B256" s="2" t="s">
@@ -4238,13 +4265,13 @@
       </c>
     </row>
     <row r="261" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B261" s="12" t="s">
+      <c r="B261" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="C261" s="13"/>
-      <c r="D261" s="13"/>
-      <c r="E261" s="13"/>
-      <c r="F261" s="14"/>
+      <c r="C261" s="19"/>
+      <c r="D261" s="19"/>
+      <c r="E261" s="19"/>
+      <c r="F261" s="20"/>
     </row>
     <row r="262" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B262" s="2" t="s">
@@ -4298,53 +4325,147 @@
       </c>
     </row>
     <row r="265" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B265" s="7">
-        <v>45870</v>
-      </c>
-      <c r="C265" s="3"/>
-      <c r="D265" s="3"/>
-      <c r="E265" s="3"/>
-      <c r="F265" s="3"/>
-    </row>
-    <row r="266" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B266" s="7">
-        <v>45871</v>
-      </c>
-      <c r="C266" s="3"/>
-      <c r="D266" s="3"/>
-      <c r="E266" s="3"/>
-      <c r="F266" s="3"/>
+      <c r="G265" s="4">
+        <f>SUM(F263:F264)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="267" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G267" s="4">
-        <f>SUM(F263:F266)</f>
-        <v>15</v>
+      <c r="B267" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="C267" s="19"/>
+      <c r="D267" s="19"/>
+      <c r="E267" s="19"/>
+      <c r="F267" s="20"/>
+    </row>
+    <row r="268" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B268" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E268" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F268" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B269" s="7">
+        <v>45873</v>
+      </c>
+      <c r="C269" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D269" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E269" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F269" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="270" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B270" s="7">
+        <v>45873</v>
+      </c>
+      <c r="C270" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D270" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E270" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F270" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="271" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B271" s="7">
+        <v>45874</v>
+      </c>
+      <c r="C271" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D271" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E271" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F271" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="272" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B272" s="7">
+        <v>45875</v>
+      </c>
+      <c r="C272" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D272" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E272" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F272" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="273" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B273" s="7">
+        <v>45876</v>
+      </c>
+      <c r="C273" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D273" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E273" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F273" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B274" s="7">
+        <v>45877</v>
+      </c>
+      <c r="C274" s="3"/>
+      <c r="D274" s="3"/>
+      <c r="E274" s="3"/>
+      <c r="F274" s="3"/>
+    </row>
+    <row r="275" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G275" s="4">
+        <f>SUM(F269:F274)</f>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B71:F71"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="B189:F189"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
+  <mergeCells count="35">
+    <mergeCell ref="B267:F267"/>
     <mergeCell ref="B249:F249"/>
     <mergeCell ref="B255:F255"/>
     <mergeCell ref="B261:F261"/>
     <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B223:F223"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B213:F213"/>
@@ -4354,9 +4475,24 @@
     <mergeCell ref="B180:F180"/>
     <mergeCell ref="B172:F172"/>
     <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B241:F241"/>
     <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B189:F189"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B125:F125"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se trabajaron cambios menores y se corrigió el desplazamiento aleatorio de las tarjetas en el modo tableta para index.html
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21E2189-57EE-4E11-8C3E-FEECC16F1975}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FAD32C-88D7-40E2-8202-D07BC22499FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="207">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -635,6 +635,18 @@
   </si>
   <si>
     <t>8:00 -12:00, 15:00 - 18:00</t>
+  </si>
+  <si>
+    <t>SEMANA 31</t>
+  </si>
+  <si>
+    <t>Se trabajó en los cambios solicitados y se corrigió un error en el modo tableta de index</t>
+  </si>
+  <si>
+    <t>Se trabajaron cambios menores y se corrigió el desplazamiento aleatorio de las tarjetas en el modo tableta para index.html</t>
+  </si>
+  <si>
+    <t>10:00 - 13:00, 15:00 - 21:00</t>
   </si>
 </sst>
 </file>
@@ -826,6 +838,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -842,15 +863,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1133,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N275"/>
+  <dimension ref="B1:N285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
-      <selection activeCell="D273" sqref="D273"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,32 +1166,32 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45876</v>
+        <v>45901</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="J5" s="16" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="J5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="16"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1197,11 +1209,11 @@
       <c r="F6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="17">
-        <f>SUM(G12:G1191)</f>
-        <v>404.2</v>
-      </c>
-      <c r="K6" s="17"/>
+      <c r="J6" s="20">
+        <f>SUM(G12:G1190)</f>
+        <v>413.2</v>
+      </c>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
@@ -1256,8 +1268,9 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>75.800000000000011</v>
-      </c>
+        <v>66.800000000000011</v>
+      </c>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
@@ -1277,7 +1290,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>18.950000000000003</v>
+        <v>16.700000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1298,7 +1311,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>0.47375000000000006</v>
+        <v>0.41750000000000009</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -1309,13 +1322,13 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -1427,13 +1440,13 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1562,13 +1575,13 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
     </row>
     <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -1680,13 +1693,13 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
     </row>
     <row r="45" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -1798,13 +1811,13 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
     </row>
     <row r="54" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -1916,13 +1929,13 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
     </row>
     <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
@@ -2034,13 +2047,13 @@
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
     </row>
     <row r="72" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
@@ -2152,13 +2165,13 @@
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
     </row>
     <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
@@ -2254,13 +2267,13 @@
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
     </row>
     <row r="90" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
@@ -2332,13 +2345,13 @@
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B98" s="12" t="s">
+      <c r="B98" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
     </row>
     <row r="99" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
@@ -2418,13 +2431,13 @@
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B107" s="12" t="s">
+      <c r="B107" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C107" s="12"/>
-      <c r="D107" s="12"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
     </row>
     <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
@@ -2520,13 +2533,13 @@
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116" s="12" t="s">
+      <c r="B116" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C116" s="12"/>
-      <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
+      <c r="C116" s="15"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
     </row>
     <row r="117" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
@@ -2622,13 +2635,13 @@
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125" s="12" t="s">
+      <c r="B125" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C125" s="12"/>
-      <c r="D125" s="12"/>
-      <c r="E125" s="12"/>
-      <c r="F125" s="12"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="15"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
     </row>
     <row r="126" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
@@ -2726,13 +2739,13 @@
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134" s="12" t="s">
+      <c r="B134" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C134" s="12"/>
-      <c r="D134" s="12"/>
-      <c r="E134" s="12"/>
-      <c r="F134" s="12"/>
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
     </row>
     <row r="135" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
@@ -2828,13 +2841,13 @@
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B143" s="12" t="s">
+      <c r="B143" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C143" s="12"/>
-      <c r="D143" s="12"/>
-      <c r="E143" s="12"/>
-      <c r="F143" s="12"/>
+      <c r="C143" s="15"/>
+      <c r="D143" s="15"/>
+      <c r="E143" s="15"/>
+      <c r="F143" s="15"/>
     </row>
     <row r="144" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
@@ -2955,13 +2968,13 @@
       <c r="N152"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B153" s="12" t="s">
+      <c r="B153" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C153" s="12"/>
-      <c r="D153" s="12"/>
-      <c r="E153" s="12"/>
-      <c r="F153" s="12"/>
+      <c r="C153" s="15"/>
+      <c r="D153" s="15"/>
+      <c r="E153" s="15"/>
+      <c r="F153" s="15"/>
       <c r="J153"/>
       <c r="K153"/>
       <c r="L153"/>
@@ -3075,13 +3088,13 @@
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B162" s="12" t="s">
+      <c r="B162" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C162" s="12"/>
-      <c r="D162" s="12"/>
-      <c r="E162" s="12"/>
-      <c r="F162" s="12"/>
+      <c r="C162" s="15"/>
+      <c r="D162" s="15"/>
+      <c r="E162" s="15"/>
+      <c r="F162" s="15"/>
     </row>
     <row r="163" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
@@ -3210,13 +3223,13 @@
       </c>
     </row>
     <row r="172" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B172" s="12" t="s">
+      <c r="B172" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C172" s="12"/>
-      <c r="D172" s="12"/>
-      <c r="E172" s="12"/>
-      <c r="F172" s="12"/>
+      <c r="C172" s="15"/>
+      <c r="D172" s="15"/>
+      <c r="E172" s="15"/>
+      <c r="F172" s="15"/>
     </row>
     <row r="173" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
@@ -3322,13 +3335,13 @@
       <c r="F179"/>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B180" s="12" t="s">
+      <c r="B180" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C180" s="12"/>
-      <c r="D180" s="12"/>
-      <c r="E180" s="12"/>
-      <c r="F180" s="12"/>
+      <c r="C180" s="15"/>
+      <c r="D180" s="15"/>
+      <c r="E180" s="15"/>
+      <c r="F180" s="15"/>
     </row>
     <row r="181" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
@@ -3448,13 +3461,13 @@
       <c r="D188" s="1"/>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="12" t="s">
+      <c r="B189" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C189" s="12"/>
-      <c r="D189" s="12"/>
-      <c r="E189" s="12"/>
-      <c r="F189" s="12"/>
+      <c r="C189" s="15"/>
+      <c r="D189" s="15"/>
+      <c r="E189" s="15"/>
+      <c r="F189" s="15"/>
     </row>
     <row r="190" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
@@ -3553,13 +3566,13 @@
       </c>
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B198" s="12" t="s">
+      <c r="B198" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C198" s="12"/>
-      <c r="D198" s="12"/>
-      <c r="E198" s="12"/>
-      <c r="F198" s="12"/>
+      <c r="C198" s="15"/>
+      <c r="D198" s="15"/>
+      <c r="E198" s="15"/>
+      <c r="F198" s="15"/>
     </row>
     <row r="199" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
@@ -3690,13 +3703,13 @@
       </c>
     </row>
     <row r="208" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B208" s="12" t="s">
+      <c r="B208" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C208" s="12"/>
-      <c r="D208" s="12"/>
-      <c r="E208" s="12"/>
-      <c r="F208" s="12"/>
+      <c r="C208" s="15"/>
+      <c r="D208" s="15"/>
+      <c r="E208" s="15"/>
+      <c r="F208" s="15"/>
     </row>
     <row r="209" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
@@ -3744,13 +3757,13 @@
       </c>
     </row>
     <row r="213" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B213" s="18" t="s">
+      <c r="B213" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C213" s="19"/>
-      <c r="D213" s="19"/>
-      <c r="E213" s="19"/>
-      <c r="F213" s="20"/>
+      <c r="C213" s="13"/>
+      <c r="D213" s="13"/>
+      <c r="E213" s="13"/>
+      <c r="F213" s="14"/>
     </row>
     <row r="214" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B214" s="2" t="s">
@@ -3808,13 +3821,13 @@
       </c>
     </row>
     <row r="218" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B218" s="18" t="s">
+      <c r="B218" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C218" s="19"/>
-      <c r="D218" s="19"/>
-      <c r="E218" s="19"/>
-      <c r="F218" s="20"/>
+      <c r="C218" s="13"/>
+      <c r="D218" s="13"/>
+      <c r="E218" s="13"/>
+      <c r="F218" s="14"/>
     </row>
     <row r="219" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B219" s="2" t="s">
@@ -3872,13 +3885,13 @@
       </c>
     </row>
     <row r="223" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B223" s="18" t="s">
+      <c r="B223" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="C223" s="19"/>
-      <c r="D223" s="19"/>
-      <c r="E223" s="19"/>
-      <c r="F223" s="20"/>
+      <c r="C223" s="13"/>
+      <c r="D223" s="13"/>
+      <c r="E223" s="13"/>
+      <c r="F223" s="14"/>
     </row>
     <row r="224" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B224" s="2" t="s">
@@ -3926,13 +3939,13 @@
       </c>
     </row>
     <row r="229" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B229" s="18" t="s">
+      <c r="B229" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C229" s="19"/>
-      <c r="D229" s="19"/>
-      <c r="E229" s="19"/>
-      <c r="F229" s="20"/>
+      <c r="C229" s="13"/>
+      <c r="D229" s="13"/>
+      <c r="E229" s="13"/>
+      <c r="F229" s="14"/>
     </row>
     <row r="230" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B230" s="2" t="s">
@@ -4067,13 +4080,13 @@
       </c>
     </row>
     <row r="241" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B241" s="18" t="s">
+      <c r="B241" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C241" s="19"/>
-      <c r="D241" s="19"/>
-      <c r="E241" s="19"/>
-      <c r="F241" s="20"/>
+      <c r="C241" s="13"/>
+      <c r="D241" s="13"/>
+      <c r="E241" s="13"/>
+      <c r="F241" s="14"/>
     </row>
     <row r="242" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B242" s="2" t="s">
@@ -4167,13 +4180,13 @@
       </c>
     </row>
     <row r="249" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B249" s="18" t="s">
+      <c r="B249" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C249" s="19"/>
-      <c r="D249" s="19"/>
-      <c r="E249" s="19"/>
-      <c r="F249" s="20"/>
+      <c r="C249" s="13"/>
+      <c r="D249" s="13"/>
+      <c r="E249" s="13"/>
+      <c r="F249" s="14"/>
     </row>
     <row r="250" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B250" s="2" t="s">
@@ -4216,13 +4229,13 @@
       </c>
     </row>
     <row r="255" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B255" s="18" t="s">
+      <c r="B255" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C255" s="19"/>
-      <c r="D255" s="19"/>
-      <c r="E255" s="19"/>
-      <c r="F255" s="20"/>
+      <c r="C255" s="13"/>
+      <c r="D255" s="13"/>
+      <c r="E255" s="13"/>
+      <c r="F255" s="14"/>
     </row>
     <row r="256" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B256" s="2" t="s">
@@ -4265,13 +4278,13 @@
       </c>
     </row>
     <row r="261" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B261" s="18" t="s">
+      <c r="B261" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C261" s="19"/>
-      <c r="D261" s="19"/>
-      <c r="E261" s="19"/>
-      <c r="F261" s="20"/>
+      <c r="C261" s="13"/>
+      <c r="D261" s="13"/>
+      <c r="E261" s="13"/>
+      <c r="F261" s="14"/>
     </row>
     <row r="262" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B262" s="2" t="s">
@@ -4331,13 +4344,13 @@
       </c>
     </row>
     <row r="267" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B267" s="18" t="s">
+      <c r="B267" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="C267" s="19"/>
-      <c r="D267" s="19"/>
-      <c r="E267" s="19"/>
-      <c r="F267" s="20"/>
+      <c r="C267" s="13"/>
+      <c r="D267" s="13"/>
+      <c r="E267" s="13"/>
+      <c r="F267" s="14"/>
     </row>
     <row r="268" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B268" s="2" t="s">
@@ -4442,30 +4455,119 @@
       </c>
     </row>
     <row r="274" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B274" s="7">
-        <v>45877</v>
-      </c>
-      <c r="C274" s="3"/>
-      <c r="D274" s="3"/>
-      <c r="E274" s="3"/>
-      <c r="F274" s="3"/>
-    </row>
-    <row r="275" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G275" s="4">
-        <f>SUM(F269:F274)</f>
+      <c r="G274" s="4">
+        <f>SUM(F269:F273)</f>
         <v>19</v>
       </c>
     </row>
+    <row r="277" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B277" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C277" s="13"/>
+      <c r="D277" s="13"/>
+      <c r="E277" s="13"/>
+      <c r="F277" s="14"/>
+    </row>
+    <row r="278" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B278" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E278" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F278" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B279" s="7">
+        <v>45901</v>
+      </c>
+      <c r="C279" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D279" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E279" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F279" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="280" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B280" s="7">
+        <v>45902</v>
+      </c>
+      <c r="C280" s="3"/>
+      <c r="D280" s="3"/>
+      <c r="E280" s="3"/>
+      <c r="F280" s="3"/>
+    </row>
+    <row r="281" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B281" s="7">
+        <v>45903</v>
+      </c>
+      <c r="C281" s="3"/>
+      <c r="D281" s="3"/>
+      <c r="E281" s="3"/>
+      <c r="F281" s="3"/>
+    </row>
+    <row r="282" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B282" s="7">
+        <v>45904</v>
+      </c>
+      <c r="C282" s="3"/>
+      <c r="D282" s="3"/>
+      <c r="E282" s="3"/>
+      <c r="F282" s="3"/>
+    </row>
+    <row r="283" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B283" s="7">
+        <v>45905</v>
+      </c>
+      <c r="C283" s="3"/>
+      <c r="D283" s="3"/>
+      <c r="E283" s="3"/>
+      <c r="F283" s="3"/>
+    </row>
+    <row r="284" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B284" s="7">
+        <v>45906</v>
+      </c>
+      <c r="C284" s="3"/>
+      <c r="D284" s="3"/>
+      <c r="E284" s="3"/>
+      <c r="F284" s="3"/>
+    </row>
+    <row r="285" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G285" s="4">
+        <f>SUM(F279:F284)</f>
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B249:F249"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B261:F261"/>
-    <mergeCell ref="B218:F218"/>
-    <mergeCell ref="B241:F241"/>
-    <mergeCell ref="B229:F229"/>
-    <mergeCell ref="B223:F223"/>
+  <mergeCells count="36">
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B213:F213"/>
@@ -4482,17 +4584,14 @@
     <mergeCell ref="B71:F71"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B189:F189"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B249:F249"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B218:F218"/>
+    <mergeCell ref="B241:F241"/>
+    <mergeCell ref="B229:F229"/>
+    <mergeCell ref="B223:F223"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se trabajó en los cambios solicitados y se corrigió un error en el modo celular en TratamientoAR.html en el navbar
</commit_message>
<xml_diff>
--- a/TABLA DE CONTROL DE ACTIVIDADES .xlsx
+++ b/TABLA DE CONTROL DE ACTIVIDADES .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ulises_Soto\Desktop\ServicioSocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FAD32C-88D7-40E2-8202-D07BC22499FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4232693B-2213-4801-A8EE-4B1E870D5D50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="209">
   <si>
     <t>ACTIVIDAD</t>
   </si>
@@ -647,6 +647,12 @@
   </si>
   <si>
     <t>10:00 - 13:00, 15:00 - 21:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se trabajó en los cambios solicitados y se corrigió un error en el modo celular en TratamientoAR.html en el navbar </t>
+  </si>
+  <si>
+    <t>9:30 - 13:00, 15:00 - 20:30</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="F282" sqref="F282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,7 +1172,7 @@
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="8">
         <f ca="1">TODAY()</f>
-        <v>45901</v>
+        <v>45930</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.25">
@@ -1211,7 +1217,7 @@
       </c>
       <c r="J6" s="20">
         <f>SUM(G12:G1190)</f>
-        <v>413.2</v>
+        <v>421.2</v>
       </c>
       <c r="K6" s="20"/>
     </row>
@@ -1268,7 +1274,7 @@
       </c>
       <c r="J9" s="11">
         <f>480-J6</f>
-        <v>66.800000000000011</v>
+        <v>58.800000000000011</v>
       </c>
       <c r="K9" s="11"/>
     </row>
@@ -1290,7 +1296,7 @@
       </c>
       <c r="J10" s="9">
         <f>+J9/4</f>
-        <v>16.700000000000003</v>
+        <v>14.700000000000003</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1311,7 +1317,7 @@
       </c>
       <c r="J11" s="9">
         <f>+J10/40</f>
-        <v>0.41750000000000009</v>
+        <v>0.36750000000000005</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -4512,14 +4518,22 @@
       <c r="E280" s="3"/>
       <c r="F280" s="3"/>
     </row>
-    <row r="281" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B281" s="7">
         <v>45903</v>
       </c>
-      <c r="C281" s="3"/>
-      <c r="D281" s="3"/>
-      <c r="E281" s="3"/>
-      <c r="F281" s="3"/>
+      <c r="C281" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D281" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E281" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F281" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="282" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B282" s="7">
@@ -4551,23 +4565,11 @@
     <row r="285" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G285" s="4">
         <f>SUM(F279:F284)</f>
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B107:F107"/>
-    <mergeCell ref="B116:F116"/>
-    <mergeCell ref="B153:F153"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B213:F213"/>
@@ -4584,6 +4586,18 @@
     <mergeCell ref="B71:F71"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B189:F189"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B116:F116"/>
+    <mergeCell ref="B153:F153"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B125:F125"/>
     <mergeCell ref="B267:F267"/>
     <mergeCell ref="B249:F249"/>
     <mergeCell ref="B255:F255"/>

</xml_diff>